<commit_message>
FIX: Site_Reference.xlsx duplicated ID and added entries as backup for domain detection
</commit_message>
<xml_diff>
--- a/common_data/Site_References_full.xlsx
+++ b/common_data/Site_References_full.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhg791/Dropbox_work/GloriamGroup Dropbox/Ismael Rodriguez Espigares/Ismael_Rodriguez_Espigares/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhg791/gpcrdb_data/common_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B620DDB-08B5-0742-831A-CEFB607F00A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CCD4CF17-CB69-1B4B-99C2-3B168C2ABAE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20620" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="References" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2255" uniqueCount="645">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2255" uniqueCount="647">
   <si>
     <t>Phylogenetic trees</t>
   </si>
@@ -1468,9 +1468,6 @@
     <t>https://gproteindb.org/mutations/gprot_coupling_*</t>
   </si>
   <si>
-    <t>42.2</t>
-  </si>
-  <si>
     <t>https://gpcrdb.org/protein/*</t>
   </si>
   <si>
@@ -1645,72 +1642,15 @@
     <t>39</t>
   </si>
   <si>
-    <t>46.2</t>
-  </si>
-  <si>
-    <t>51.2</t>
-  </si>
-  <si>
-    <t>51.3</t>
-  </si>
-  <si>
-    <t>54.2</t>
-  </si>
-  <si>
-    <t>54.3</t>
-  </si>
-  <si>
-    <t>55.2</t>
-  </si>
-  <si>
-    <t>57.1</t>
-  </si>
-  <si>
-    <t>58.1.2</t>
-  </si>
-  <si>
-    <t>58.1.3</t>
-  </si>
-  <si>
-    <t>60.2</t>
-  </si>
-  <si>
-    <t>60.3</t>
-  </si>
-  <si>
-    <t>61.2</t>
-  </si>
-  <si>
-    <t>63.2.1</t>
-  </si>
-  <si>
-    <t>63.2.2</t>
-  </si>
-  <si>
-    <t>64.1</t>
-  </si>
-  <si>
     <t>64.2</t>
   </si>
   <si>
-    <t>64.*</t>
-  </si>
-  <si>
     <t>65</t>
   </si>
   <si>
-    <t>65.2</t>
-  </si>
-  <si>
-    <t>65.3</t>
-  </si>
-  <si>
     <t>66</t>
   </si>
   <si>
-    <t>66.2</t>
-  </si>
-  <si>
     <t>68</t>
   </si>
   <si>
@@ -1720,9 +1660,6 @@
     <t>68.3</t>
   </si>
   <si>
-    <t>68.4</t>
-  </si>
-  <si>
     <t>69</t>
   </si>
   <si>
@@ -1735,27 +1672,18 @@
     <t>70</t>
   </si>
   <si>
-    <t>70.2</t>
-  </si>
-  <si>
     <t>71</t>
   </si>
   <si>
     <t>71.2</t>
   </si>
   <si>
-    <t>72.3</t>
-  </si>
-  <si>
     <t>73</t>
   </si>
   <si>
     <t>73.2</t>
   </si>
   <si>
-    <t>73.3</t>
-  </si>
-  <si>
     <t>74</t>
   </si>
   <si>
@@ -1765,12 +1693,6 @@
     <t>75.2</t>
   </si>
   <si>
-    <t>75.2.1</t>
-  </si>
-  <si>
-    <t>75.2.2</t>
-  </si>
-  <si>
     <t>75.3</t>
   </si>
   <si>
@@ -1789,12 +1711,6 @@
     <t>80</t>
   </si>
   <si>
-    <t>80.2</t>
-  </si>
-  <si>
-    <t>80.3</t>
-  </si>
-  <si>
     <t>81</t>
   </si>
   <si>
@@ -1804,9 +1720,6 @@
     <t>82.2</t>
   </si>
   <si>
-    <t>82.2.2</t>
-  </si>
-  <si>
     <t>83</t>
   </si>
   <si>
@@ -1838,18 +1751,6 @@
   </si>
   <si>
     <t>92</t>
-  </si>
-  <si>
-    <t>92.2</t>
-  </si>
-  <si>
-    <t>92.3</t>
-  </si>
-  <si>
-    <t>92.4</t>
-  </si>
-  <si>
-    <t>92.4.2</t>
   </si>
   <si>
     <t>93</t>
@@ -2044,6 +1945,111 @@
   </si>
   <si>
     <t>https://doi.org/10.1038/s41589-023-01292-8</t>
+  </si>
+  <si>
+    <t>43.2</t>
+  </si>
+  <si>
+    <t>49.2</t>
+  </si>
+  <si>
+    <t>57.2</t>
+  </si>
+  <si>
+    <t>60.1</t>
+  </si>
+  <si>
+    <t>57.3</t>
+  </si>
+  <si>
+    <t>58.2</t>
+  </si>
+  <si>
+    <t>61.1.2</t>
+  </si>
+  <si>
+    <t>61.1.3</t>
+  </si>
+  <si>
+    <t>63.2</t>
+  </si>
+  <si>
+    <t>63.3</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>66.2.1</t>
+  </si>
+  <si>
+    <t>66.2.2</t>
+  </si>
+  <si>
+    <t>67.1</t>
+  </si>
+  <si>
+    <t>67.2</t>
+  </si>
+  <si>
+    <t>67.*</t>
+  </si>
+  <si>
+    <t>71.3</t>
+  </si>
+  <si>
+    <t>71.4</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
+    <t>72.2</t>
+  </si>
+  <si>
+    <t>74.2</t>
+  </si>
+  <si>
+    <t>74.3</t>
+  </si>
+  <si>
+    <t>77.2</t>
+  </si>
+  <si>
+    <t>77.2.1</t>
+  </si>
+  <si>
+    <t>77.2.2</t>
+  </si>
+  <si>
+    <t>77.3</t>
+  </si>
+  <si>
+    <t>82.3</t>
+  </si>
+  <si>
+    <t>84.2.2</t>
+  </si>
+  <si>
+    <t>86.2</t>
+  </si>
+  <si>
+    <t>94</t>
+  </si>
+  <si>
+    <t>94.2</t>
+  </si>
+  <si>
+    <t>94.3</t>
+  </si>
+  <si>
+    <t>94.4</t>
+  </si>
+  <si>
+    <t>94.4.2</t>
+  </si>
+  <si>
+    <t>95</t>
   </si>
 </sst>
 </file>
@@ -2933,9 +2939,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF192"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17:XFD17"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A109" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A122" sqref="A122:XFD122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2943,7 +2949,7 @@
     <col min="1" max="1" width="9.33203125" style="28" customWidth="1"/>
     <col min="2" max="2" width="8" customWidth="1"/>
     <col min="3" max="3" width="10.1640625" style="14" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" style="14" customWidth="1"/>
+    <col min="4" max="4" width="19" style="14" customWidth="1"/>
     <col min="5" max="5" width="50" style="14" customWidth="1"/>
     <col min="6" max="6" width="50.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="43.1640625" customWidth="1"/>
@@ -3010,34 +3016,34 @@
         <v>126</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>618</v>
+        <v>585</v>
       </c>
       <c r="Q1" s="60" t="s">
-        <v>607</v>
+        <v>574</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>608</v>
+        <v>575</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>609</v>
+        <v>576</v>
       </c>
       <c r="T1" s="5" t="s">
-        <v>610</v>
+        <v>577</v>
       </c>
       <c r="U1" s="5" t="s">
-        <v>617</v>
+        <v>584</v>
       </c>
       <c r="V1" s="6" t="s">
-        <v>619</v>
+        <v>586</v>
       </c>
       <c r="W1" s="5" t="s">
-        <v>620</v>
+        <v>587</v>
       </c>
       <c r="X1" s="5" t="s">
-        <v>621</v>
+        <v>588</v>
       </c>
       <c r="Y1" s="5" t="s">
-        <v>622</v>
+        <v>589</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
@@ -3079,13 +3085,13 @@
         <v>37</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="H3" s="1" t="b">
         <v>1</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>603</v>
+        <v>570</v>
       </c>
       <c r="K3" s="16" t="s">
         <v>177</v>
@@ -3115,7 +3121,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="J4" s="1" t="s">
-        <v>603</v>
+        <v>570</v>
       </c>
       <c r="K4" s="16" t="s">
         <v>177</v>
@@ -3145,7 +3151,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="J5" s="1" t="s">
-        <v>603</v>
+        <v>570</v>
       </c>
       <c r="K5" s="16" t="s">
         <v>177</v>
@@ -3175,7 +3181,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="J6" s="1" t="s">
-        <v>603</v>
+        <v>570</v>
       </c>
       <c r="K6" s="16" t="s">
         <v>177</v>
@@ -3205,7 +3211,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="J7" s="1" t="s">
-        <v>603</v>
+        <v>570</v>
       </c>
       <c r="K7" s="16" t="s">
         <v>177</v>
@@ -3235,7 +3241,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="J8" s="1" t="s">
-        <v>603</v>
+        <v>570</v>
       </c>
       <c r="K8" s="16" t="s">
         <v>177</v>
@@ -3265,7 +3271,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="J9" s="1" t="s">
-        <v>603</v>
+        <v>570</v>
       </c>
       <c r="K9" s="16" t="s">
         <v>177</v>
@@ -3295,7 +3301,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="J10" s="1" t="s">
-        <v>603</v>
+        <v>570</v>
       </c>
       <c r="K10" s="16" t="s">
         <v>177</v>
@@ -3325,7 +3331,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="J11" s="1" t="s">
-        <v>603</v>
+        <v>570</v>
       </c>
       <c r="K11" s="16" t="s">
         <v>177</v>
@@ -3355,7 +3361,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="J12" s="1" t="s">
-        <v>603</v>
+        <v>570</v>
       </c>
       <c r="K12" s="16" t="s">
         <v>177</v>
@@ -3385,7 +3391,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="J13" s="1" t="s">
-        <v>603</v>
+        <v>570</v>
       </c>
       <c r="K13" s="16" t="s">
         <v>177</v>
@@ -3415,7 +3421,7 @@
         <v>468</v>
       </c>
       <c r="J14" s="41" t="s">
-        <v>603</v>
+        <v>570</v>
       </c>
       <c r="K14" s="41" t="s">
         <v>177</v>
@@ -3447,7 +3453,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="J15" s="1" t="s">
-        <v>603</v>
+        <v>570</v>
       </c>
       <c r="K15" s="16" t="s">
         <v>177</v>
@@ -3476,7 +3482,7 @@
       </c>
       <c r="H16" s="22"/>
       <c r="J16" s="1" t="s">
-        <v>603</v>
+        <v>570</v>
       </c>
       <c r="K16" s="16" t="s">
         <v>177</v>
@@ -5134,19 +5140,19 @@
         <v>84</v>
       </c>
       <c r="P71" s="1" t="s">
-        <v>614</v>
+        <v>581</v>
       </c>
       <c r="Q71" s="9" t="s">
         <v>77</v>
       </c>
       <c r="R71" t="s">
-        <v>615</v>
+        <v>582</v>
       </c>
       <c r="S71">
         <v>2025</v>
       </c>
       <c r="T71" t="s">
-        <v>616</v>
+        <v>583</v>
       </c>
     </row>
     <row r="72" spans="1:24" x14ac:dyDescent="0.2">
@@ -5191,13 +5197,13 @@
         <v>84</v>
       </c>
       <c r="P72" s="1" t="s">
-        <v>630</v>
+        <v>597</v>
       </c>
       <c r="Q72" s="9" t="s">
         <v>77</v>
       </c>
       <c r="R72" t="s">
-        <v>629</v>
+        <v>596</v>
       </c>
       <c r="S72">
         <v>2023</v>
@@ -5205,7 +5211,7 @@
     </row>
     <row r="73" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A73" s="28" t="s">
-        <v>641</v>
+        <v>608</v>
       </c>
       <c r="B73" s="49"/>
       <c r="D73" s="49"/>
@@ -5235,25 +5241,25 @@
         <v>84</v>
       </c>
       <c r="P73" s="1" t="s">
-        <v>630</v>
+        <v>597</v>
       </c>
       <c r="Q73" s="9" t="s">
         <v>77</v>
       </c>
       <c r="R73" t="s">
-        <v>629</v>
+        <v>596</v>
       </c>
       <c r="S73">
         <v>2023</v>
       </c>
       <c r="U73" s="1" t="s">
-        <v>633</v>
+        <v>600</v>
       </c>
       <c r="V73" s="9" t="s">
-        <v>635</v>
+        <v>602</v>
       </c>
       <c r="W73" t="s">
-        <v>634</v>
+        <v>601</v>
       </c>
       <c r="X73">
         <v>2025</v>
@@ -5261,7 +5267,7 @@
     </row>
     <row r="74" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A74" s="28" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B74" s="49" t="s">
         <v>203</v>
@@ -5301,13 +5307,13 @@
         <v>84</v>
       </c>
       <c r="P74" s="1" t="s">
-        <v>630</v>
+        <v>597</v>
       </c>
       <c r="Q74" s="9" t="s">
         <v>77</v>
       </c>
       <c r="R74" t="s">
-        <v>629</v>
+        <v>596</v>
       </c>
       <c r="S74">
         <v>2023</v>
@@ -5355,13 +5361,13 @@
         <v>84</v>
       </c>
       <c r="P75" s="1" t="s">
-        <v>630</v>
+        <v>597</v>
       </c>
       <c r="Q75" s="9" t="s">
         <v>77</v>
       </c>
       <c r="R75" t="s">
-        <v>629</v>
+        <v>596</v>
       </c>
       <c r="S75">
         <v>2023</v>
@@ -5391,7 +5397,7 @@
       </c>
       <c r="H76" s="1"/>
       <c r="J76" s="1" t="s">
-        <v>614</v>
+        <v>581</v>
       </c>
       <c r="K76" s="16" t="s">
         <v>179</v>
@@ -5400,18 +5406,18 @@
         <v>77</v>
       </c>
       <c r="M76" t="s">
-        <v>615</v>
+        <v>582</v>
       </c>
       <c r="N76">
         <v>2025</v>
       </c>
       <c r="O76" t="s">
-        <v>616</v>
+        <v>583</v>
       </c>
     </row>
     <row r="77" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A77" s="28" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B77" s="49" t="s">
         <v>203</v>
@@ -5433,7 +5439,7 @@
       </c>
       <c r="H77" s="1"/>
       <c r="J77" s="1" t="s">
-        <v>614</v>
+        <v>581</v>
       </c>
       <c r="K77" s="16" t="s">
         <v>179</v>
@@ -5442,18 +5448,18 @@
         <v>77</v>
       </c>
       <c r="M77" t="s">
-        <v>615</v>
+        <v>582</v>
       </c>
       <c r="N77">
         <v>2025</v>
       </c>
       <c r="O77" t="s">
-        <v>616</v>
+        <v>583</v>
       </c>
     </row>
     <row r="78" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A78" s="28" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B78" s="49" t="s">
         <v>203</v>
@@ -5470,7 +5476,7 @@
       </c>
       <c r="H78" s="1"/>
       <c r="J78" s="1" t="s">
-        <v>614</v>
+        <v>581</v>
       </c>
       <c r="K78" s="16" t="s">
         <v>179</v>
@@ -5479,18 +5485,18 @@
         <v>77</v>
       </c>
       <c r="M78" t="s">
-        <v>615</v>
+        <v>582</v>
       </c>
       <c r="N78">
         <v>2025</v>
       </c>
       <c r="O78" t="s">
-        <v>616</v>
+        <v>583</v>
       </c>
     </row>
     <row r="79" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A79" s="28" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B79" s="49" t="s">
         <v>203</v>
@@ -5527,13 +5533,13 @@
         <v>2017</v>
       </c>
       <c r="P79" s="1" t="s">
-        <v>633</v>
+        <v>600</v>
       </c>
       <c r="Q79" s="9" t="s">
-        <v>635</v>
+        <v>602</v>
       </c>
       <c r="R79" t="s">
-        <v>634</v>
+        <v>601</v>
       </c>
       <c r="S79">
         <v>2025</v>
@@ -5541,7 +5547,7 @@
     </row>
     <row r="80" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A80" s="28" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B80" s="49" t="s">
         <v>203</v>
@@ -5578,13 +5584,13 @@
         <v>2017</v>
       </c>
       <c r="P80" s="1" t="s">
-        <v>633</v>
+        <v>600</v>
       </c>
       <c r="Q80" s="9" t="s">
-        <v>635</v>
+        <v>602</v>
       </c>
       <c r="R80" t="s">
-        <v>634</v>
+        <v>601</v>
       </c>
       <c r="S80">
         <v>2025</v>
@@ -5592,7 +5598,7 @@
     </row>
     <row r="81" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A81" s="28" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B81" s="49" t="s">
         <v>203</v>
@@ -5629,13 +5635,13 @@
         <v>2017</v>
       </c>
       <c r="P81" s="1" t="s">
-        <v>633</v>
+        <v>600</v>
       </c>
       <c r="Q81" s="9" t="s">
-        <v>635</v>
+        <v>602</v>
       </c>
       <c r="R81" t="s">
-        <v>634</v>
+        <v>601</v>
       </c>
       <c r="S81">
         <v>2025</v>
@@ -5643,7 +5649,7 @@
     </row>
     <row r="82" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A82" s="28" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B82" s="49" t="s">
         <v>203</v>
@@ -5661,7 +5667,7 @@
         <v>435</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="H82" s="46"/>
       <c r="J82" s="1" t="s">
@@ -5680,13 +5686,13 @@
         <v>2017</v>
       </c>
       <c r="P82" s="1" t="s">
-        <v>633</v>
+        <v>600</v>
       </c>
       <c r="Q82" s="9" t="s">
-        <v>635</v>
+        <v>602</v>
       </c>
       <c r="R82" t="s">
-        <v>634</v>
+        <v>601</v>
       </c>
       <c r="S82">
         <v>2025</v>
@@ -5694,7 +5700,7 @@
     </row>
     <row r="83" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A83" s="28" t="s">
-        <v>373</v>
+        <v>531</v>
       </c>
       <c r="B83" s="49" t="s">
         <v>203</v>
@@ -5731,13 +5737,13 @@
         <v>2017</v>
       </c>
       <c r="P83" s="1" t="s">
-        <v>633</v>
+        <v>600</v>
       </c>
       <c r="Q83" s="9" t="s">
-        <v>635</v>
+        <v>602</v>
       </c>
       <c r="R83" t="s">
-        <v>634</v>
+        <v>601</v>
       </c>
       <c r="S83">
         <v>2025</v>
@@ -5745,7 +5751,7 @@
     </row>
     <row r="84" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A84" s="28" t="s">
-        <v>532</v>
+        <v>374</v>
       </c>
       <c r="B84" s="49" t="s">
         <v>203</v>
@@ -5782,13 +5788,13 @@
         <v>2017</v>
       </c>
       <c r="P84" s="1" t="s">
-        <v>633</v>
+        <v>600</v>
       </c>
       <c r="Q84" s="9" t="s">
-        <v>635</v>
+        <v>602</v>
       </c>
       <c r="R84" t="s">
-        <v>634</v>
+        <v>601</v>
       </c>
       <c r="S84">
         <v>2025</v>
@@ -5796,7 +5802,7 @@
     </row>
     <row r="85" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A85" s="28" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B85" s="49" t="s">
         <v>203</v>
@@ -5833,13 +5839,13 @@
         <v>2017</v>
       </c>
       <c r="P85" s="1" t="s">
-        <v>633</v>
+        <v>600</v>
       </c>
       <c r="Q85" s="9" t="s">
-        <v>635</v>
+        <v>602</v>
       </c>
       <c r="R85" t="s">
-        <v>634</v>
+        <v>601</v>
       </c>
       <c r="S85">
         <v>2025</v>
@@ -5847,7 +5853,7 @@
     </row>
     <row r="86" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A86" s="28" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B86" s="49" t="s">
         <v>203</v>
@@ -5884,13 +5890,13 @@
         <v>2017</v>
       </c>
       <c r="P86" s="1" t="s">
-        <v>633</v>
+        <v>600</v>
       </c>
       <c r="Q86" s="9" t="s">
-        <v>635</v>
+        <v>602</v>
       </c>
       <c r="R86" t="s">
-        <v>634</v>
+        <v>601</v>
       </c>
       <c r="S86">
         <v>2025</v>
@@ -5898,7 +5904,7 @@
     </row>
     <row r="87" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A87" s="28" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B87" s="49" t="s">
         <v>203</v>
@@ -5958,7 +5964,7 @@
     </row>
     <row r="88" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A88" s="28" t="s">
-        <v>474</v>
+        <v>612</v>
       </c>
       <c r="B88" s="49" t="s">
         <v>203</v>
@@ -5976,7 +5982,7 @@
         <v>16</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>627</v>
+        <v>594</v>
       </c>
       <c r="H88" s="1" t="b">
         <v>1</v>
@@ -6018,7 +6024,7 @@
     </row>
     <row r="89" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A89" s="28" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B89" s="49" t="s">
         <v>203</v>
@@ -6060,7 +6066,7 @@
     </row>
     <row r="90" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A90" s="28" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B90" s="49" t="s">
         <v>203</v>
@@ -6105,7 +6111,7 @@
     </row>
     <row r="91" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A91" s="28" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B91" s="49" t="s">
         <v>203</v>
@@ -6144,7 +6150,7 @@
     </row>
     <row r="92" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="28" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B92" s="49" t="s">
         <v>203</v>
@@ -6186,7 +6192,7 @@
     </row>
     <row r="93" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="28" t="s">
-        <v>533</v>
+        <v>458</v>
       </c>
       <c r="B93" s="49" t="s">
         <v>203</v>
@@ -6201,7 +6207,7 @@
         <v>90</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="H93" s="1"/>
       <c r="I93" s="2"/>
@@ -6226,7 +6232,7 @@
     </row>
     <row r="94" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A94" s="28" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="B94" s="49" t="s">
         <v>203</v>
@@ -6268,7 +6274,7 @@
     </row>
     <row r="95" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A95" s="28" t="s">
-        <v>458</v>
+        <v>472</v>
       </c>
       <c r="B95" s="49" t="s">
         <v>203</v>
@@ -6286,7 +6292,7 @@
         <v>174</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="H95" s="1"/>
       <c r="J95" s="1" t="s">
@@ -6310,7 +6316,7 @@
     </row>
     <row r="96" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A96" s="28" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B96" s="49" t="s">
         <v>203</v>
@@ -6352,7 +6358,7 @@
     </row>
     <row r="97" spans="1:24" s="41" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A97" s="40" t="s">
-        <v>472</v>
+        <v>613</v>
       </c>
       <c r="B97" s="50" t="s">
         <v>203</v>
@@ -6370,7 +6376,7 @@
         <v>173</v>
       </c>
       <c r="G97" s="41" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="J97" s="41" t="s">
         <v>116</v>
@@ -6394,7 +6400,7 @@
     </row>
     <row r="98" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A98" s="28" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B98" s="51" t="s">
         <v>203</v>
@@ -6435,7 +6441,7 @@
     </row>
     <row r="99" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A99" s="28" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B99" s="49" t="s">
         <v>178</v>
@@ -6468,7 +6474,7 @@
     </row>
     <row r="100" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A100" s="28" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B100" s="49" t="s">
         <v>178</v>
@@ -6487,7 +6493,7 @@
       </c>
       <c r="H100" s="1"/>
       <c r="J100" s="1" t="s">
-        <v>636</v>
+        <v>603</v>
       </c>
       <c r="K100" s="16" t="s">
         <v>178</v>
@@ -6496,19 +6502,19 @@
         <v>77</v>
       </c>
       <c r="M100" t="s">
-        <v>637</v>
+        <v>604</v>
       </c>
       <c r="N100">
         <v>2024</v>
       </c>
       <c r="P100" s="1" t="s">
-        <v>638</v>
+        <v>605</v>
       </c>
       <c r="Q100" s="9" t="s">
-        <v>639</v>
+        <v>606</v>
       </c>
       <c r="R100" t="s">
-        <v>640</v>
+        <v>607</v>
       </c>
       <c r="S100">
         <v>2022</v>
@@ -6528,7 +6534,7 @@
     </row>
     <row r="101" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A101" s="28" t="s">
-        <v>534</v>
+        <v>387</v>
       </c>
       <c r="B101" s="49" t="s">
         <v>178</v>
@@ -6548,7 +6554,7 @@
       </c>
       <c r="H101" s="1"/>
       <c r="J101" s="1" t="s">
-        <v>636</v>
+        <v>603</v>
       </c>
       <c r="K101" s="16" t="s">
         <v>178</v>
@@ -6557,19 +6563,19 @@
         <v>77</v>
       </c>
       <c r="M101" t="s">
-        <v>637</v>
+        <v>604</v>
       </c>
       <c r="N101">
         <v>2024</v>
       </c>
       <c r="P101" s="1" t="s">
-        <v>638</v>
+        <v>605</v>
       </c>
       <c r="Q101" s="9" t="s">
-        <v>639</v>
+        <v>606</v>
       </c>
       <c r="R101" t="s">
-        <v>640</v>
+        <v>607</v>
       </c>
       <c r="S101">
         <v>2022</v>
@@ -6589,7 +6595,7 @@
     </row>
     <row r="102" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A102" s="28" t="s">
-        <v>535</v>
+        <v>388</v>
       </c>
       <c r="B102" s="49" t="s">
         <v>178</v>
@@ -6608,7 +6614,7 @@
       </c>
       <c r="H102" s="1"/>
       <c r="J102" s="1" t="s">
-        <v>636</v>
+        <v>603</v>
       </c>
       <c r="K102" s="16" t="s">
         <v>178</v>
@@ -6617,19 +6623,19 @@
         <v>77</v>
       </c>
       <c r="M102" t="s">
-        <v>637</v>
+        <v>604</v>
       </c>
       <c r="N102">
         <v>2024</v>
       </c>
       <c r="P102" s="1" t="s">
-        <v>638</v>
+        <v>605</v>
       </c>
       <c r="Q102" s="9" t="s">
-        <v>639</v>
+        <v>606</v>
       </c>
       <c r="R102" t="s">
-        <v>640</v>
+        <v>607</v>
       </c>
       <c r="S102">
         <v>2022</v>
@@ -6649,7 +6655,7 @@
     </row>
     <row r="103" spans="1:24" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="28" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="B103" s="49" t="s">
         <v>178</v>
@@ -6677,7 +6683,7 @@
     </row>
     <row r="104" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A104" s="28" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="B104" s="49" t="s">
         <v>178</v>
@@ -6705,7 +6711,7 @@
     </row>
     <row r="105" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A105" s="28" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="B105" s="49" t="s">
         <v>178</v>
@@ -6741,7 +6747,7 @@
     </row>
     <row r="106" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A106" s="28" t="s">
-        <v>536</v>
+        <v>614</v>
       </c>
       <c r="B106" s="49" t="s">
         <v>178</v>
@@ -6777,7 +6783,7 @@
     </row>
     <row r="107" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A107" s="28" t="s">
-        <v>537</v>
+        <v>616</v>
       </c>
       <c r="B107" s="49" t="s">
         <v>178</v>
@@ -6813,7 +6819,7 @@
     </row>
     <row r="108" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A108" s="28" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="B108" s="49" t="s">
         <v>178</v>
@@ -6849,7 +6855,7 @@
     </row>
     <row r="109" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A109" s="28" t="s">
-        <v>538</v>
+        <v>617</v>
       </c>
       <c r="B109" s="49" t="s">
         <v>178</v>
@@ -6887,7 +6893,7 @@
     </row>
     <row r="110" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A110" s="28" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="B110" s="49" t="s">
         <v>178</v>
@@ -6906,7 +6912,7 @@
       </c>
       <c r="H110" s="1"/>
       <c r="J110" s="1" t="s">
-        <v>636</v>
+        <v>603</v>
       </c>
       <c r="K110" s="16" t="s">
         <v>178</v>
@@ -6915,7 +6921,7 @@
         <v>77</v>
       </c>
       <c r="M110" t="s">
-        <v>637</v>
+        <v>604</v>
       </c>
       <c r="N110">
         <v>2024</v>
@@ -6935,7 +6941,7 @@
     </row>
     <row r="111" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A111" s="28" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="B111" s="49" t="s">
         <v>178</v>
@@ -6954,7 +6960,7 @@
       </c>
       <c r="H111" s="1"/>
       <c r="J111" s="1" t="s">
-        <v>636</v>
+        <v>603</v>
       </c>
       <c r="K111" s="16" t="s">
         <v>178</v>
@@ -6963,7 +6969,7 @@
         <v>77</v>
       </c>
       <c r="M111" t="s">
-        <v>637</v>
+        <v>604</v>
       </c>
       <c r="N111">
         <v>2024</v>
@@ -6983,7 +6989,7 @@
     </row>
     <row r="112" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A112" s="28" t="s">
-        <v>539</v>
+        <v>615</v>
       </c>
       <c r="B112" s="49" t="s">
         <v>178</v>
@@ -7002,7 +7008,7 @@
       </c>
       <c r="H112" s="1"/>
       <c r="J112" s="1" t="s">
-        <v>636</v>
+        <v>603</v>
       </c>
       <c r="K112" s="16" t="s">
         <v>178</v>
@@ -7011,7 +7017,7 @@
         <v>77</v>
       </c>
       <c r="M112" t="s">
-        <v>637</v>
+        <v>604</v>
       </c>
       <c r="N112">
         <v>2024</v>
@@ -7031,7 +7037,7 @@
     </row>
     <row r="113" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A113" s="28" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="B113" s="49" t="s">
         <v>178</v>
@@ -7050,7 +7056,7 @@
       </c>
       <c r="H113" s="1"/>
       <c r="J113" s="1" t="s">
-        <v>636</v>
+        <v>603</v>
       </c>
       <c r="K113" s="16" t="s">
         <v>178</v>
@@ -7059,7 +7065,7 @@
         <v>77</v>
       </c>
       <c r="M113" t="s">
-        <v>637</v>
+        <v>604</v>
       </c>
       <c r="N113">
         <v>2024</v>
@@ -7069,7 +7075,7 @@
     </row>
     <row r="114" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A114" s="28" t="s">
-        <v>540</v>
+        <v>618</v>
       </c>
       <c r="B114" s="49" t="s">
         <v>178</v>
@@ -7105,7 +7111,7 @@
     </row>
     <row r="115" spans="1:20" s="41" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A115" s="40" t="s">
-        <v>541</v>
+        <v>619</v>
       </c>
       <c r="B115" s="50" t="s">
         <v>178</v>
@@ -7142,7 +7148,7 @@
     </row>
     <row r="116" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="28" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="B116" s="49" t="s">
         <v>178</v>
@@ -7178,7 +7184,7 @@
     </row>
     <row r="117" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="28" t="s">
-        <v>394</v>
+        <v>407</v>
       </c>
       <c r="B117" s="49" t="s">
         <v>178</v>
@@ -7214,7 +7220,7 @@
     </row>
     <row r="118" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="28" t="s">
-        <v>542</v>
+        <v>620</v>
       </c>
       <c r="B118" s="49" t="s">
         <v>178</v>
@@ -7250,7 +7256,7 @@
     </row>
     <row r="119" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="28" t="s">
-        <v>543</v>
+        <v>621</v>
       </c>
       <c r="B119" s="49" t="s">
         <v>178</v>
@@ -7286,7 +7292,7 @@
     </row>
     <row r="120" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A120" s="28" t="s">
-        <v>395</v>
+        <v>622</v>
       </c>
       <c r="B120" s="49" t="s">
         <v>178</v>
@@ -7322,7 +7328,7 @@
     </row>
     <row r="121" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A121" s="28" t="s">
-        <v>544</v>
+        <v>532</v>
       </c>
       <c r="B121" s="49" t="s">
         <v>178</v>
@@ -7360,7 +7366,7 @@
     </row>
     <row r="122" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A122" s="29" t="s">
-        <v>396</v>
+        <v>533</v>
       </c>
       <c r="B122" s="51" t="s">
         <v>178</v>
@@ -7402,7 +7408,7 @@
     </row>
     <row r="123" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="28" t="s">
-        <v>407</v>
+        <v>534</v>
       </c>
       <c r="B123" s="49" t="s">
         <v>179</v>
@@ -7439,24 +7445,24 @@
         <v>78</v>
       </c>
       <c r="P123" s="1" t="s">
-        <v>611</v>
+        <v>578</v>
       </c>
       <c r="Q123" s="9" t="s">
         <v>77</v>
       </c>
       <c r="R123" t="s">
-        <v>612</v>
+        <v>579</v>
       </c>
       <c r="S123">
         <v>2014</v>
       </c>
       <c r="T123" t="s">
-        <v>613</v>
+        <v>580</v>
       </c>
     </row>
     <row r="124" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="28" t="s">
-        <v>545</v>
+        <v>623</v>
       </c>
       <c r="B124" s="49" t="s">
         <v>179</v>
@@ -7469,7 +7475,7 @@
         <v>129</v>
       </c>
       <c r="G124" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="H124" s="1" t="b">
         <v>1</v>
@@ -7494,34 +7500,34 @@
         <v>78</v>
       </c>
       <c r="P124" s="1" t="s">
-        <v>611</v>
+        <v>578</v>
       </c>
       <c r="Q124" s="9" t="s">
         <v>77</v>
       </c>
       <c r="R124" t="s">
-        <v>612</v>
+        <v>579</v>
       </c>
       <c r="S124">
         <v>2014</v>
       </c>
       <c r="T124" t="s">
-        <v>613</v>
+        <v>580</v>
       </c>
     </row>
     <row r="125" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="28" t="s">
-        <v>546</v>
+        <v>624</v>
       </c>
       <c r="B125" s="49" t="s">
         <v>179</v>
       </c>
       <c r="D125" s="49"/>
       <c r="F125" t="s">
-        <v>561</v>
+        <v>540</v>
       </c>
       <c r="G125" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="H125" s="1" t="b">
         <v>1</v>
@@ -7546,42 +7552,42 @@
         <v>78</v>
       </c>
       <c r="P125" s="1" t="s">
-        <v>611</v>
+        <v>578</v>
       </c>
       <c r="Q125" s="9" t="s">
         <v>77</v>
       </c>
       <c r="R125" t="s">
-        <v>612</v>
+        <v>579</v>
       </c>
       <c r="S125">
         <v>2014</v>
       </c>
       <c r="T125" t="s">
-        <v>613</v>
+        <v>580</v>
       </c>
     </row>
     <row r="126" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="28" t="s">
-        <v>547</v>
+        <v>625</v>
       </c>
       <c r="B126" s="49" t="s">
         <v>179</v>
       </c>
       <c r="D126" s="49"/>
       <c r="E126" s="14" t="s">
+        <v>477</v>
+      </c>
+      <c r="F126" t="s">
         <v>478</v>
       </c>
-      <c r="F126" t="s">
-        <v>479</v>
-      </c>
       <c r="G126" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="H126" s="1"/>
       <c r="I126" s="2"/>
       <c r="J126" s="1" t="s">
-        <v>614</v>
+        <v>581</v>
       </c>
       <c r="K126" s="16" t="s">
         <v>179</v>
@@ -7590,34 +7596,34 @@
         <v>77</v>
       </c>
       <c r="M126" t="s">
-        <v>615</v>
+        <v>582</v>
       </c>
       <c r="N126">
         <v>2025</v>
       </c>
       <c r="O126" t="s">
-        <v>616</v>
+        <v>583</v>
       </c>
     </row>
     <row r="127" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A127" s="28" t="s">
-        <v>548</v>
+        <v>626</v>
       </c>
       <c r="B127" s="49" t="s">
         <v>179</v>
       </c>
       <c r="D127" s="49"/>
       <c r="E127" s="14" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="F127" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="G127" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="J127" s="1" t="s">
-        <v>614</v>
+        <v>581</v>
       </c>
       <c r="K127" s="16" t="s">
         <v>179</v>
@@ -7626,34 +7632,34 @@
         <v>77</v>
       </c>
       <c r="M127" t="s">
-        <v>615</v>
+        <v>582</v>
       </c>
       <c r="N127">
         <v>2025</v>
       </c>
       <c r="O127" t="s">
-        <v>616</v>
+        <v>583</v>
       </c>
     </row>
     <row r="128" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A128" s="28" t="s">
-        <v>549</v>
+        <v>627</v>
       </c>
       <c r="B128" s="49" t="s">
         <v>179</v>
       </c>
       <c r="D128" s="49"/>
       <c r="E128" s="14" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="G128" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="H128" t="b">
         <v>1</v>
       </c>
       <c r="J128" s="1" t="s">
-        <v>614</v>
+        <v>581</v>
       </c>
       <c r="K128" s="16" t="s">
         <v>179</v>
@@ -7662,18 +7668,18 @@
         <v>77</v>
       </c>
       <c r="M128" t="s">
-        <v>615</v>
+        <v>582</v>
       </c>
       <c r="N128">
         <v>2025</v>
       </c>
       <c r="O128" t="s">
-        <v>616</v>
+        <v>583</v>
       </c>
     </row>
     <row r="129" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A129" s="28" t="s">
-        <v>550</v>
+        <v>535</v>
       </c>
       <c r="B129" s="49" t="s">
         <v>179</v>
@@ -7713,7 +7719,7 @@
         <v>78</v>
       </c>
       <c r="P129" s="1" t="s">
-        <v>623</v>
+        <v>590</v>
       </c>
       <c r="Q129" s="9" t="s">
         <v>77</v>
@@ -7725,12 +7731,12 @@
         <v>2021</v>
       </c>
       <c r="T129" t="s">
-        <v>628</v>
+        <v>595</v>
       </c>
     </row>
     <row r="130" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A130" s="28" t="s">
-        <v>551</v>
+        <v>536</v>
       </c>
       <c r="B130" s="49" t="s">
         <v>179</v>
@@ -7745,7 +7751,7 @@
         <v>30</v>
       </c>
       <c r="G130" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="H130" s="1"/>
       <c r="I130" s="2"/>
@@ -7768,7 +7774,7 @@
         <v>78</v>
       </c>
       <c r="P130" s="1" t="s">
-        <v>623</v>
+        <v>590</v>
       </c>
       <c r="Q130" s="9" t="s">
         <v>77</v>
@@ -7780,12 +7786,12 @@
         <v>2021</v>
       </c>
       <c r="T130" t="s">
-        <v>628</v>
+        <v>595</v>
       </c>
     </row>
     <row r="131" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A131" s="28" t="s">
-        <v>552</v>
+        <v>537</v>
       </c>
       <c r="B131" s="49" t="s">
         <v>179</v>
@@ -7800,7 +7806,7 @@
         <v>30</v>
       </c>
       <c r="G131" s="1" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="H131" s="1"/>
       <c r="I131" s="2"/>
@@ -7823,7 +7829,7 @@
         <v>78</v>
       </c>
       <c r="P131" s="1" t="s">
-        <v>623</v>
+        <v>590</v>
       </c>
       <c r="Q131" s="9" t="s">
         <v>77</v>
@@ -7835,12 +7841,12 @@
         <v>2021</v>
       </c>
       <c r="T131" t="s">
-        <v>628</v>
+        <v>595</v>
       </c>
     </row>
     <row r="132" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A132" s="28" t="s">
-        <v>553</v>
+        <v>538</v>
       </c>
       <c r="B132" s="49" t="s">
         <v>179</v>
@@ -7877,13 +7883,13 @@
         <v>78</v>
       </c>
       <c r="P132" s="1" t="s">
-        <v>624</v>
+        <v>591</v>
       </c>
       <c r="Q132" s="9" t="s">
         <v>86</v>
       </c>
       <c r="R132" t="s">
-        <v>625</v>
+        <v>592</v>
       </c>
       <c r="S132">
         <v>2015</v>
@@ -7894,7 +7900,7 @@
     </row>
     <row r="133" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A133" s="28" t="s">
-        <v>554</v>
+        <v>539</v>
       </c>
       <c r="B133" s="49" t="s">
         <v>179</v>
@@ -7909,7 +7915,7 @@
         <v>130</v>
       </c>
       <c r="G133" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="H133" s="1"/>
       <c r="I133" s="2"/>
@@ -7932,13 +7938,13 @@
         <v>78</v>
       </c>
       <c r="P133" s="1" t="s">
-        <v>624</v>
+        <v>591</v>
       </c>
       <c r="Q133" s="9" t="s">
         <v>86</v>
       </c>
       <c r="R133" t="s">
-        <v>625</v>
+        <v>592</v>
       </c>
       <c r="S133">
         <v>2015</v>
@@ -7949,7 +7955,7 @@
     </row>
     <row r="134" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A134" s="28" t="s">
-        <v>397</v>
+        <v>541</v>
       </c>
       <c r="B134" s="49" t="s">
         <v>179</v>
@@ -7988,7 +7994,7 @@
     </row>
     <row r="135" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A135" s="28" t="s">
-        <v>555</v>
+        <v>542</v>
       </c>
       <c r="B135" s="49" t="s">
         <v>179</v>
@@ -7997,10 +8003,10 @@
         <v>165</v>
       </c>
       <c r="D135" s="49" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E135" s="14" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="F135" t="s">
         <v>131</v>
@@ -8037,7 +8043,7 @@
         <v>81</v>
       </c>
       <c r="R135" t="s">
-        <v>626</v>
+        <v>593</v>
       </c>
       <c r="S135">
         <v>2016</v>
@@ -8064,7 +8070,7 @@
     </row>
     <row r="136" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A136" s="28" t="s">
-        <v>556</v>
+        <v>543</v>
       </c>
       <c r="B136" s="49" t="s">
         <v>179</v>
@@ -8073,16 +8079,16 @@
         <v>165</v>
       </c>
       <c r="D136" s="49" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E136" s="14" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="F136" t="s">
         <v>131</v>
       </c>
       <c r="G136" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="H136" s="1"/>
       <c r="I136" s="2"/>
@@ -8111,7 +8117,7 @@
         <v>81</v>
       </c>
       <c r="R136" t="s">
-        <v>626</v>
+        <v>593</v>
       </c>
       <c r="S136">
         <v>2016</v>
@@ -8122,7 +8128,7 @@
     </row>
     <row r="137" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A137" s="28" t="s">
-        <v>557</v>
+        <v>628</v>
       </c>
       <c r="B137" s="49" t="s">
         <v>179</v>
@@ -8131,16 +8137,16 @@
         <v>165</v>
       </c>
       <c r="D137" s="49" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E137" s="14" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="F137" t="s">
         <v>131</v>
       </c>
       <c r="G137" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H137" s="1"/>
       <c r="I137" s="2"/>
@@ -8169,7 +8175,7 @@
         <v>81</v>
       </c>
       <c r="R137" t="s">
-        <v>626</v>
+        <v>593</v>
       </c>
       <c r="S137">
         <v>2016</v>
@@ -8180,7 +8186,7 @@
     </row>
     <row r="138" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A138" s="28" t="s">
-        <v>558</v>
+        <v>629</v>
       </c>
       <c r="B138" s="49" t="s">
         <v>179</v>
@@ -8189,16 +8195,16 @@
         <v>165</v>
       </c>
       <c r="D138" s="49" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E138" s="14" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="F138" t="s">
         <v>131</v>
       </c>
       <c r="G138" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H138" s="1"/>
       <c r="I138" s="2"/>
@@ -8227,7 +8233,7 @@
         <v>81</v>
       </c>
       <c r="R138" t="s">
-        <v>626</v>
+        <v>593</v>
       </c>
       <c r="S138">
         <v>2016</v>
@@ -8238,7 +8244,7 @@
     </row>
     <row r="139" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A139" s="28" t="s">
-        <v>559</v>
+        <v>630</v>
       </c>
       <c r="B139" s="49" t="s">
         <v>179</v>
@@ -8247,10 +8253,10 @@
         <v>165</v>
       </c>
       <c r="D139" s="49" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E139" s="14" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="F139" t="s">
         <v>132</v>
@@ -8284,7 +8290,7 @@
         <v>81</v>
       </c>
       <c r="R139" t="s">
-        <v>626</v>
+        <v>593</v>
       </c>
       <c r="S139">
         <v>2016</v>
@@ -8295,7 +8301,7 @@
     </row>
     <row r="140" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A140" s="28" t="s">
-        <v>560</v>
+        <v>631</v>
       </c>
       <c r="B140" s="49" t="s">
         <v>179</v>
@@ -8304,16 +8310,16 @@
         <v>165</v>
       </c>
       <c r="D140" s="49" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E140" s="14" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="F140" t="s">
         <v>132</v>
       </c>
       <c r="G140" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="H140" s="1"/>
       <c r="J140" s="1" t="s">
@@ -8341,7 +8347,7 @@
         <v>81</v>
       </c>
       <c r="R140" t="s">
-        <v>626</v>
+        <v>593</v>
       </c>
       <c r="S140">
         <v>2016</v>
@@ -8352,7 +8358,7 @@
     </row>
     <row r="141" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A141" s="28" t="s">
-        <v>562</v>
+        <v>544</v>
       </c>
       <c r="B141" s="49" t="s">
         <v>179</v>
@@ -8361,10 +8367,10 @@
         <v>165</v>
       </c>
       <c r="D141" s="49" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E141" s="14" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="F141" t="s">
         <v>0</v>
@@ -8398,7 +8404,7 @@
         <v>81</v>
       </c>
       <c r="R141" t="s">
-        <v>626</v>
+        <v>593</v>
       </c>
       <c r="S141">
         <v>2016</v>
@@ -8409,7 +8415,7 @@
     </row>
     <row r="142" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A142" s="28" t="s">
-        <v>563</v>
+        <v>545</v>
       </c>
       <c r="B142" s="49" t="s">
         <v>179</v>
@@ -8418,16 +8424,16 @@
         <v>165</v>
       </c>
       <c r="D142" s="49" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E142" s="14" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="F142" t="s">
         <v>0</v>
       </c>
       <c r="G142" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="H142" s="1"/>
       <c r="J142" s="1" t="s">
@@ -8455,7 +8461,7 @@
         <v>81</v>
       </c>
       <c r="R142" t="s">
-        <v>626</v>
+        <v>593</v>
       </c>
       <c r="S142">
         <v>2016</v>
@@ -8466,7 +8472,7 @@
     </row>
     <row r="143" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A143" s="28" t="s">
-        <v>564</v>
+        <v>546</v>
       </c>
       <c r="B143" s="49" t="s">
         <v>179</v>
@@ -8475,10 +8481,10 @@
         <v>165</v>
       </c>
       <c r="D143" s="49" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E143" s="14" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="F143" t="s">
         <v>133</v>
@@ -8512,7 +8518,7 @@
         <v>81</v>
       </c>
       <c r="R143" t="s">
-        <v>626</v>
+        <v>593</v>
       </c>
       <c r="S143">
         <v>2016</v>
@@ -8523,7 +8529,7 @@
     </row>
     <row r="144" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A144" s="28" t="s">
-        <v>565</v>
+        <v>632</v>
       </c>
       <c r="B144" s="49" t="s">
         <v>179</v>
@@ -8532,16 +8538,16 @@
         <v>165</v>
       </c>
       <c r="D144" s="49" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E144" s="14" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="F144" t="s">
         <v>133</v>
       </c>
       <c r="G144" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="H144" s="1"/>
       <c r="J144" s="1" t="s">
@@ -8569,7 +8575,7 @@
         <v>81</v>
       </c>
       <c r="R144" t="s">
-        <v>626</v>
+        <v>593</v>
       </c>
       <c r="S144">
         <v>2016</v>
@@ -8580,7 +8586,7 @@
     </row>
     <row r="145" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A145" s="28" t="s">
-        <v>566</v>
+        <v>633</v>
       </c>
       <c r="B145" s="49" t="s">
         <v>179</v>
@@ -8589,16 +8595,16 @@
         <v>165</v>
       </c>
       <c r="D145" s="49" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E145" s="14" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="F145" t="s">
         <v>133</v>
       </c>
       <c r="G145" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H145" s="1"/>
       <c r="J145" s="1" t="s">
@@ -8626,7 +8632,7 @@
         <v>81</v>
       </c>
       <c r="R145" t="s">
-        <v>626</v>
+        <v>593</v>
       </c>
       <c r="S145">
         <v>2016</v>
@@ -8637,7 +8643,7 @@
     </row>
     <row r="146" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A146" s="28" t="s">
-        <v>567</v>
+        <v>547</v>
       </c>
       <c r="B146" s="49" t="s">
         <v>179</v>
@@ -8646,7 +8652,7 @@
         <v>165</v>
       </c>
       <c r="D146" s="49" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F146" t="s">
         <v>134</v>
@@ -8676,7 +8682,7 @@
     </row>
     <row r="147" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A147" s="28" t="s">
-        <v>568</v>
+        <v>548</v>
       </c>
       <c r="B147" s="49" t="s">
         <v>179</v>
@@ -8685,13 +8691,13 @@
         <v>165</v>
       </c>
       <c r="D147" s="49" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F147" t="s">
         <v>134</v>
       </c>
       <c r="G147" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="J147" s="1" t="s">
         <v>114</v>
@@ -8714,7 +8720,7 @@
     </row>
     <row r="148" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A148" s="28" t="s">
-        <v>569</v>
+        <v>549</v>
       </c>
       <c r="B148" s="49" t="s">
         <v>179</v>
@@ -8723,13 +8729,13 @@
         <v>165</v>
       </c>
       <c r="D148" s="49" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F148" t="s">
         <v>134</v>
       </c>
       <c r="G148" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="J148" s="1" t="s">
         <v>114</v>
@@ -8752,7 +8758,7 @@
     </row>
     <row r="149" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A149" s="28" t="s">
-        <v>570</v>
+        <v>550</v>
       </c>
       <c r="B149" s="49" t="s">
         <v>179</v>
@@ -8794,7 +8800,7 @@
     </row>
     <row r="150" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A150" s="28" t="s">
-        <v>571</v>
+        <v>551</v>
       </c>
       <c r="B150" s="49" t="s">
         <v>179</v>
@@ -8828,27 +8834,27 @@
         <v>2021</v>
       </c>
       <c r="O150" t="s">
-        <v>628</v>
+        <v>595</v>
       </c>
       <c r="P150" s="1" t="s">
-        <v>611</v>
+        <v>578</v>
       </c>
       <c r="Q150" s="9" t="s">
         <v>77</v>
       </c>
       <c r="R150" t="s">
-        <v>612</v>
+        <v>579</v>
       </c>
       <c r="S150">
         <v>2014</v>
       </c>
       <c r="T150" t="s">
-        <v>613</v>
+        <v>580</v>
       </c>
     </row>
     <row r="151" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A151" s="28" t="s">
-        <v>572</v>
+        <v>634</v>
       </c>
       <c r="B151" s="49" t="s">
         <v>179</v>
@@ -8860,10 +8866,10 @@
         <v>31</v>
       </c>
       <c r="F151" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G151" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="H151" s="1"/>
       <c r="J151" s="1" t="s">
@@ -8882,27 +8888,27 @@
         <v>2021</v>
       </c>
       <c r="O151" t="s">
-        <v>628</v>
+        <v>595</v>
       </c>
       <c r="P151" s="1" t="s">
-        <v>611</v>
+        <v>578</v>
       </c>
       <c r="Q151" s="9" t="s">
         <v>77</v>
       </c>
       <c r="R151" t="s">
-        <v>612</v>
+        <v>579</v>
       </c>
       <c r="S151">
         <v>2014</v>
       </c>
       <c r="T151" t="s">
-        <v>613</v>
+        <v>580</v>
       </c>
     </row>
     <row r="152" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A152" s="28" t="s">
-        <v>573</v>
+        <v>635</v>
       </c>
       <c r="B152" s="49" t="s">
         <v>179</v>
@@ -8914,10 +8920,10 @@
         <v>31</v>
       </c>
       <c r="F152" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="G152" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="H152" s="1"/>
       <c r="J152" s="1" t="s">
@@ -8936,27 +8942,27 @@
         <v>2021</v>
       </c>
       <c r="O152" t="s">
-        <v>628</v>
+        <v>595</v>
       </c>
       <c r="P152" s="1" t="s">
-        <v>611</v>
+        <v>578</v>
       </c>
       <c r="Q152" s="9" t="s">
         <v>77</v>
       </c>
       <c r="R152" t="s">
-        <v>612</v>
+        <v>579</v>
       </c>
       <c r="S152">
         <v>2014</v>
       </c>
       <c r="T152" t="s">
-        <v>613</v>
+        <v>580</v>
       </c>
     </row>
     <row r="153" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A153" s="28" t="s">
-        <v>574</v>
+        <v>636</v>
       </c>
       <c r="B153" s="49" t="s">
         <v>179</v>
@@ -8968,10 +8974,10 @@
         <v>31</v>
       </c>
       <c r="F153" t="s">
+        <v>515</v>
+      </c>
+      <c r="G153" s="1" t="s">
         <v>516</v>
-      </c>
-      <c r="G153" s="1" t="s">
-        <v>517</v>
       </c>
       <c r="H153" s="1"/>
       <c r="J153" s="1" t="s">
@@ -8990,27 +8996,27 @@
         <v>2021</v>
       </c>
       <c r="O153" t="s">
-        <v>628</v>
+        <v>595</v>
       </c>
       <c r="P153" s="1" t="s">
-        <v>611</v>
+        <v>578</v>
       </c>
       <c r="Q153" s="9" t="s">
         <v>77</v>
       </c>
       <c r="R153" t="s">
-        <v>612</v>
+        <v>579</v>
       </c>
       <c r="S153">
         <v>2014</v>
       </c>
       <c r="T153" t="s">
-        <v>613</v>
+        <v>580</v>
       </c>
     </row>
     <row r="154" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A154" s="28" t="s">
-        <v>575</v>
+        <v>637</v>
       </c>
       <c r="B154" s="49" t="s">
         <v>179</v>
@@ -9022,10 +9028,10 @@
         <v>31</v>
       </c>
       <c r="F154" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G154" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="H154" s="1"/>
       <c r="J154" s="1" t="s">
@@ -9044,22 +9050,22 @@
         <v>2021</v>
       </c>
       <c r="O154" t="s">
-        <v>628</v>
+        <v>595</v>
       </c>
       <c r="P154" s="1" t="s">
-        <v>611</v>
+        <v>578</v>
       </c>
       <c r="Q154" s="9" t="s">
         <v>77</v>
       </c>
       <c r="R154" t="s">
-        <v>612</v>
+        <v>579</v>
       </c>
       <c r="S154">
         <v>2014</v>
       </c>
       <c r="T154" t="s">
-        <v>613</v>
+        <v>580</v>
       </c>
       <c r="U154" s="1" t="s">
         <v>114</v>
@@ -9082,7 +9088,7 @@
     </row>
     <row r="155" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A155" s="28" t="s">
-        <v>576</v>
+        <v>552</v>
       </c>
       <c r="B155" s="49" t="s">
         <v>179</v>
@@ -9094,14 +9100,14 @@
         <v>31</v>
       </c>
       <c r="F155" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="G155" s="1" t="s">
         <v>49</v>
       </c>
       <c r="H155" s="1"/>
       <c r="J155" s="1" t="s">
-        <v>630</v>
+        <v>597</v>
       </c>
       <c r="K155" s="16" t="s">
         <v>179</v>
@@ -9110,7 +9116,7 @@
         <v>77</v>
       </c>
       <c r="M155" t="s">
-        <v>629</v>
+        <v>596</v>
       </c>
       <c r="N155">
         <v>2023</v>
@@ -9118,7 +9124,7 @@
     </row>
     <row r="156" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A156" s="28" t="s">
-        <v>577</v>
+        <v>553</v>
       </c>
       <c r="B156" s="49" t="s">
         <v>179</v>
@@ -9130,14 +9136,14 @@
         <v>31</v>
       </c>
       <c r="F156" t="s">
+        <v>507</v>
+      </c>
+      <c r="G156" s="1" t="s">
         <v>508</v>
-      </c>
-      <c r="G156" s="1" t="s">
-        <v>509</v>
       </c>
       <c r="H156" s="1"/>
       <c r="J156" s="1" t="s">
-        <v>614</v>
+        <v>581</v>
       </c>
       <c r="K156" s="16" t="s">
         <v>179</v>
@@ -9146,18 +9152,18 @@
         <v>77</v>
       </c>
       <c r="M156" t="s">
-        <v>615</v>
+        <v>582</v>
       </c>
       <c r="N156">
         <v>2025</v>
       </c>
       <c r="O156" t="s">
-        <v>616</v>
+        <v>583</v>
       </c>
     </row>
     <row r="157" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A157" s="28" t="s">
-        <v>578</v>
+        <v>554</v>
       </c>
       <c r="B157" s="49" t="s">
         <v>179</v>
@@ -9166,7 +9172,7 @@
         <v>157</v>
       </c>
       <c r="D157" s="52" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F157" t="s">
         <v>159</v>
@@ -9199,7 +9205,7 @@
     </row>
     <row r="158" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A158" s="28" t="s">
-        <v>579</v>
+        <v>555</v>
       </c>
       <c r="B158" s="49" t="s">
         <v>179</v>
@@ -9208,7 +9214,7 @@
         <v>157</v>
       </c>
       <c r="D158" s="52" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F158" t="s">
         <v>163</v>
@@ -9241,7 +9247,7 @@
     </row>
     <row r="159" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A159" s="28" t="s">
-        <v>580</v>
+        <v>556</v>
       </c>
       <c r="B159" s="49" t="s">
         <v>179</v>
@@ -9250,7 +9256,7 @@
         <v>157</v>
       </c>
       <c r="D159" s="52" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F159" t="s">
         <v>7</v>
@@ -9280,7 +9286,7 @@
     </row>
     <row r="160" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A160" s="28" t="s">
-        <v>581</v>
+        <v>557</v>
       </c>
       <c r="B160" s="49" t="s">
         <v>179</v>
@@ -9289,13 +9295,13 @@
         <v>157</v>
       </c>
       <c r="D160" s="52" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F160" t="s">
         <v>7</v>
       </c>
       <c r="G160" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="H160" s="1"/>
       <c r="J160" s="1" t="s">
@@ -9319,7 +9325,7 @@
     </row>
     <row r="161" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A161" s="28" t="s">
-        <v>582</v>
+        <v>638</v>
       </c>
       <c r="B161" s="49" t="s">
         <v>179</v>
@@ -9328,13 +9334,13 @@
         <v>157</v>
       </c>
       <c r="D161" s="52" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F161" t="s">
         <v>7</v>
       </c>
       <c r="G161" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="H161" s="1"/>
       <c r="J161" s="1" t="s">
@@ -9358,7 +9364,7 @@
     </row>
     <row r="162" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A162" s="28" t="s">
-        <v>583</v>
+        <v>558</v>
       </c>
       <c r="B162" s="49" t="s">
         <v>179</v>
@@ -9367,13 +9373,13 @@
         <v>157</v>
       </c>
       <c r="D162" s="52" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F162" t="s">
+        <v>527</v>
+      </c>
+      <c r="G162" s="1" t="s">
         <v>528</v>
-      </c>
-      <c r="G162" s="1" t="s">
-        <v>529</v>
       </c>
       <c r="H162" s="1"/>
       <c r="J162" s="1" t="s">
@@ -9397,7 +9403,7 @@
     </row>
     <row r="163" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A163" s="28" t="s">
-        <v>584</v>
+        <v>559</v>
       </c>
       <c r="B163" s="49" t="s">
         <v>179</v>
@@ -9406,7 +9412,7 @@
         <v>157</v>
       </c>
       <c r="D163" s="52" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F163" t="s">
         <v>136</v>
@@ -9451,7 +9457,7 @@
     </row>
     <row r="164" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A164" s="28" t="s">
-        <v>585</v>
+        <v>560</v>
       </c>
       <c r="B164" s="49" t="s">
         <v>179</v>
@@ -9460,13 +9466,13 @@
         <v>157</v>
       </c>
       <c r="D164" s="52" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F164" t="s">
         <v>136</v>
       </c>
       <c r="G164" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="H164" s="1"/>
       <c r="J164" s="1" t="s">
@@ -9490,7 +9496,7 @@
     </row>
     <row r="165" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A165" s="28" t="s">
-        <v>586</v>
+        <v>639</v>
       </c>
       <c r="B165" s="49" t="s">
         <v>179</v>
@@ -9499,13 +9505,13 @@
         <v>157</v>
       </c>
       <c r="D165" s="52" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F165" t="s">
         <v>136</v>
       </c>
       <c r="G165" s="1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="H165" s="1"/>
       <c r="J165" s="1" t="s">
@@ -9529,7 +9535,7 @@
     </row>
     <row r="166" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A166" s="28" t="s">
-        <v>587</v>
+        <v>561</v>
       </c>
       <c r="B166" s="49" t="s">
         <v>179</v>
@@ -9541,7 +9547,7 @@
         <v>20</v>
       </c>
       <c r="E166" s="14" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F166" t="s">
         <v>21</v>
@@ -9571,7 +9577,7 @@
     </row>
     <row r="167" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A167" s="28" t="s">
-        <v>588</v>
+        <v>562</v>
       </c>
       <c r="B167" s="49" t="s">
         <v>179</v>
@@ -9583,7 +9589,7 @@
         <v>20</v>
       </c>
       <c r="E167" s="14" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F167" t="s">
         <v>22</v>
@@ -9616,7 +9622,7 @@
     </row>
     <row r="168" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A168" s="28" t="s">
-        <v>589</v>
+        <v>640</v>
       </c>
       <c r="B168" s="49" t="s">
         <v>179</v>
@@ -9628,13 +9634,13 @@
         <v>20</v>
       </c>
       <c r="E168" s="14" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F168" t="s">
         <v>22</v>
       </c>
       <c r="G168" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="H168" s="1"/>
       <c r="I168" s="1"/>
@@ -9659,7 +9665,7 @@
     </row>
     <row r="169" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A169" s="28" t="s">
-        <v>590</v>
+        <v>563</v>
       </c>
       <c r="B169" s="49" t="s">
         <v>179</v>
@@ -9671,7 +9677,7 @@
         <v>20</v>
       </c>
       <c r="E169" s="14" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F169" t="s">
         <v>24</v>
@@ -9701,7 +9707,7 @@
     </row>
     <row r="170" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A170" s="28" t="s">
-        <v>591</v>
+        <v>564</v>
       </c>
       <c r="B170" s="49" t="s">
         <v>179</v>
@@ -9713,7 +9719,7 @@
         <v>20</v>
       </c>
       <c r="E170" s="14" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="F170" t="s">
         <v>25</v>
@@ -9745,7 +9751,7 @@
     </row>
     <row r="171" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A171" s="28" t="s">
-        <v>592</v>
+        <v>565</v>
       </c>
       <c r="B171" s="49" t="s">
         <v>179</v>
@@ -9757,7 +9763,7 @@
         <v>20</v>
       </c>
       <c r="E171" s="14" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="F171" t="s">
         <v>26</v>
@@ -9789,7 +9795,7 @@
     </row>
     <row r="172" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A172" s="28" t="s">
-        <v>593</v>
+        <v>566</v>
       </c>
       <c r="B172" s="49" t="s">
         <v>179</v>
@@ -9801,7 +9807,7 @@
         <v>20</v>
       </c>
       <c r="E172" s="14" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="F172" t="s">
         <v>27</v>
@@ -9833,7 +9839,7 @@
     </row>
     <row r="173" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A173" s="28" t="s">
-        <v>594</v>
+        <v>567</v>
       </c>
       <c r="B173" s="49" t="s">
         <v>179</v>
@@ -9845,7 +9851,7 @@
         <v>20</v>
       </c>
       <c r="E173" s="14" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F173" t="s">
         <v>176</v>
@@ -9875,7 +9881,7 @@
     </row>
     <row r="174" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A174" s="28" t="s">
-        <v>595</v>
+        <v>568</v>
       </c>
       <c r="B174" s="49" t="s">
         <v>179</v>
@@ -9887,7 +9893,7 @@
         <v>20</v>
       </c>
       <c r="E174" s="14" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F174" t="s">
         <v>28</v>
@@ -9917,7 +9923,7 @@
     </row>
     <row r="175" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A175" s="28" t="s">
-        <v>596</v>
+        <v>569</v>
       </c>
       <c r="B175" s="49" t="s">
         <v>179</v>
@@ -9929,7 +9935,7 @@
         <v>20</v>
       </c>
       <c r="E175" s="14" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F175" t="s">
         <v>29</v>
@@ -9959,7 +9965,7 @@
     </row>
     <row r="176" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A176" s="28" t="s">
-        <v>597</v>
+        <v>641</v>
       </c>
       <c r="B176" s="49" t="s">
         <v>179</v>
@@ -9993,12 +9999,12 @@
         <v>2021</v>
       </c>
       <c r="O176" t="s">
-        <v>628</v>
+        <v>595</v>
       </c>
     </row>
     <row r="177" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A177" s="28" t="s">
-        <v>598</v>
+        <v>642</v>
       </c>
       <c r="B177" s="49" t="s">
         <v>179</v>
@@ -10013,7 +10019,7 @@
         <v>166</v>
       </c>
       <c r="G177" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H177" s="1"/>
       <c r="J177" s="1" t="s">
@@ -10032,12 +10038,12 @@
         <v>2021</v>
       </c>
       <c r="O177" t="s">
-        <v>628</v>
+        <v>595</v>
       </c>
     </row>
     <row r="178" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A178" s="28" t="s">
-        <v>599</v>
+        <v>643</v>
       </c>
       <c r="B178" s="49" t="s">
         <v>179</v>
@@ -10052,7 +10058,7 @@
         <v>166</v>
       </c>
       <c r="G178" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H178" s="1"/>
       <c r="J178" s="1" t="s">
@@ -10071,12 +10077,12 @@
         <v>2021</v>
       </c>
       <c r="O178" t="s">
-        <v>628</v>
+        <v>595</v>
       </c>
     </row>
     <row r="179" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A179" s="28" t="s">
-        <v>600</v>
+        <v>644</v>
       </c>
       <c r="B179" s="49" t="s">
         <v>179</v>
@@ -10091,7 +10097,7 @@
         <v>166</v>
       </c>
       <c r="G179" s="1" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="H179" s="1"/>
       <c r="J179" s="1" t="s">
@@ -10110,12 +10116,12 @@
         <v>2021</v>
       </c>
       <c r="O179" t="s">
-        <v>628</v>
+        <v>595</v>
       </c>
     </row>
     <row r="180" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A180" s="28" t="s">
-        <v>601</v>
+        <v>645</v>
       </c>
       <c r="B180" s="49" t="s">
         <v>179</v>
@@ -10130,7 +10136,7 @@
         <v>166</v>
       </c>
       <c r="G180" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="H180" s="1" t="b">
         <v>1</v>
@@ -10151,12 +10157,12 @@
         <v>2021</v>
       </c>
       <c r="O180" t="s">
-        <v>628</v>
+        <v>595</v>
       </c>
     </row>
     <row r="181" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A181" s="28" t="s">
-        <v>602</v>
+        <v>646</v>
       </c>
       <c r="B181" s="49" t="s">
         <v>179</v>
@@ -10168,7 +10174,7 @@
         <v>158</v>
       </c>
       <c r="F181" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="G181" s="1" t="s">
         <v>167</v>
@@ -10195,7 +10201,7 @@
     </row>
     <row r="182" spans="1:15" x14ac:dyDescent="0.2">
       <c r="G182" s="1" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="J182" s="1" t="s">
         <v>201</v>
@@ -10609,6 +10615,7 @@
     <hyperlink ref="J113" r:id="rId326" xr:uid="{5DA7D1EB-82AE-A143-9882-FD9307B2ACF8}"/>
     <hyperlink ref="J114" r:id="rId327" xr:uid="{4851288B-2FA3-DF4F-B4E1-64E0454F72EA}"/>
     <hyperlink ref="J121" r:id="rId328" xr:uid="{8EC2A773-9B2E-C54C-A8F8-019A9DAB3BED}"/>
+    <hyperlink ref="G9" r:id="rId329" xr:uid="{1A65AF54-92AE-794F-A0C2-2246662AB79A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10618,7 +10625,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFA36285-19E8-D244-9D5D-ABE845366A0D}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -10639,7 +10646,7 @@
         <v>75</v>
       </c>
       <c r="B1" s="53" t="s">
-        <v>643</v>
+        <v>610</v>
       </c>
       <c r="C1" s="66" t="s">
         <v>127</v>
@@ -10660,10 +10667,10 @@
         <v>126</v>
       </c>
       <c r="I1" s="68" t="s">
-        <v>604</v>
+        <v>571</v>
       </c>
       <c r="J1" s="68" t="s">
-        <v>605</v>
+        <v>572</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -10674,7 +10681,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="65" t="s">
-        <v>603</v>
+        <v>570</v>
       </c>
       <c r="D2" s="48" t="s">
         <v>177</v>
@@ -10683,7 +10690,7 @@
         <v>215</v>
       </c>
       <c r="F2" s="59" t="s">
-        <v>642</v>
+        <v>609</v>
       </c>
       <c r="G2" s="59"/>
       <c r="H2" s="59"/>
@@ -10691,7 +10698,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="54" t="s">
-        <v>606</v>
+        <v>573</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -10702,16 +10709,16 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>644</v>
+        <v>611</v>
       </c>
       <c r="D3" s="48" t="s">
         <v>216</v>
       </c>
       <c r="E3" s="59" t="s">
-        <v>631</v>
+        <v>598</v>
       </c>
       <c r="F3" s="59" t="s">
-        <v>632</v>
+        <v>599</v>
       </c>
       <c r="G3" s="59">
         <v>2023</v>
@@ -10728,7 +10735,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="65" t="s">
-        <v>614</v>
+        <v>581</v>
       </c>
       <c r="D4" s="48" t="s">
         <v>179</v>
@@ -10737,13 +10744,13 @@
         <v>77</v>
       </c>
       <c r="F4" s="59" t="s">
-        <v>615</v>
+        <v>582</v>
       </c>
       <c r="G4" s="59">
         <v>2025</v>
       </c>
       <c r="H4" s="59" t="s">
-        <v>616</v>
+        <v>583</v>
       </c>
       <c r="I4" s="59"/>
       <c r="J4" s="59"/>
@@ -10756,7 +10763,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>636</v>
+        <v>603</v>
       </c>
       <c r="D5" s="48" t="s">
         <v>178</v>
@@ -10765,7 +10772,7 @@
         <v>77</v>
       </c>
       <c r="F5" s="59" t="s">
-        <v>637</v>
+        <v>604</v>
       </c>
       <c r="G5" s="59">
         <v>2024</v>
@@ -10808,16 +10815,16 @@
         <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>638</v>
+        <v>605</v>
       </c>
       <c r="D7" s="48" t="s">
         <v>178</v>
       </c>
       <c r="E7" s="69" t="s">
-        <v>639</v>
+        <v>606</v>
       </c>
       <c r="F7" s="59" t="s">
-        <v>640</v>
+        <v>607</v>
       </c>
       <c r="G7" s="59">
         <v>2022</v>

</xml_diff>

<commit_message>
FIX: typo in Site_references_full.xlsx
</commit_message>
<xml_diff>
--- a/common_data/Site_References_full.xlsx
+++ b/common_data/Site_References_full.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhg791/gpcrdb_data/common_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CCD4CF17-CB69-1B4B-99C2-3B168C2ABAE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{870E2C59-E6AA-7E46-9A13-1C57422B4BF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="References" sheetId="1" r:id="rId1"/>
@@ -1472,9 +1472,6 @@
   </si>
   <si>
     <t>https://arrestindb.org/signprot/*</t>
-  </si>
-  <si>
-    <t>https://gpcrdb.org/familiy/*</t>
   </si>
   <si>
     <t>Data maper</t>
@@ -2050,6 +2047,9 @@
   </si>
   <si>
     <t>95</t>
+  </si>
+  <si>
+    <t>https://gpcrdb.org/family/*</t>
   </si>
 </sst>
 </file>
@@ -2941,7 +2941,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A109" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A122" sqref="A122:XFD122"/>
+      <selection pane="bottomLeft" activeCell="G125" sqref="G125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3016,34 +3016,34 @@
         <v>126</v>
       </c>
       <c r="P1" s="5" t="s">
+        <v>584</v>
+      </c>
+      <c r="Q1" s="60" t="s">
+        <v>573</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>574</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>575</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>576</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>583</v>
+      </c>
+      <c r="V1" s="6" t="s">
         <v>585</v>
       </c>
-      <c r="Q1" s="60" t="s">
-        <v>574</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>575</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>576</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>577</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>584</v>
-      </c>
-      <c r="V1" s="6" t="s">
+      <c r="W1" s="5" t="s">
         <v>586</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>587</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>588</v>
-      </c>
-      <c r="Y1" s="5" t="s">
-        <v>589</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
@@ -3091,7 +3091,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="K3" s="16" t="s">
         <v>177</v>
@@ -3121,7 +3121,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="J4" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="K4" s="16" t="s">
         <v>177</v>
@@ -3151,7 +3151,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="J5" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="K5" s="16" t="s">
         <v>177</v>
@@ -3181,7 +3181,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="J6" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="K6" s="16" t="s">
         <v>177</v>
@@ -3211,7 +3211,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="J7" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="K7" s="16" t="s">
         <v>177</v>
@@ -3241,7 +3241,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="J8" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="K8" s="16" t="s">
         <v>177</v>
@@ -3271,7 +3271,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="J9" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="K9" s="16" t="s">
         <v>177</v>
@@ -3301,7 +3301,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="J10" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="K10" s="16" t="s">
         <v>177</v>
@@ -3331,7 +3331,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="J11" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="K11" s="16" t="s">
         <v>177</v>
@@ -3361,7 +3361,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="J12" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="K12" s="16" t="s">
         <v>177</v>
@@ -3391,7 +3391,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="J13" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="K13" s="16" t="s">
         <v>177</v>
@@ -3421,7 +3421,7 @@
         <v>468</v>
       </c>
       <c r="J14" s="41" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="K14" s="41" t="s">
         <v>177</v>
@@ -3453,7 +3453,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="J15" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="K15" s="16" t="s">
         <v>177</v>
@@ -3482,7 +3482,7 @@
       </c>
       <c r="H16" s="22"/>
       <c r="J16" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="K16" s="16" t="s">
         <v>177</v>
@@ -5140,19 +5140,19 @@
         <v>84</v>
       </c>
       <c r="P71" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="Q71" s="9" t="s">
         <v>77</v>
       </c>
       <c r="R71" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="S71">
         <v>2025</v>
       </c>
       <c r="T71" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="72" spans="1:24" x14ac:dyDescent="0.2">
@@ -5197,13 +5197,13 @@
         <v>84</v>
       </c>
       <c r="P72" s="1" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="Q72" s="9" t="s">
         <v>77</v>
       </c>
       <c r="R72" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="S72">
         <v>2023</v>
@@ -5211,7 +5211,7 @@
     </row>
     <row r="73" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A73" s="28" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B73" s="49"/>
       <c r="D73" s="49"/>
@@ -5241,25 +5241,25 @@
         <v>84</v>
       </c>
       <c r="P73" s="1" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="Q73" s="9" t="s">
         <v>77</v>
       </c>
       <c r="R73" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="S73">
         <v>2023</v>
       </c>
       <c r="U73" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="V73" s="9" t="s">
+        <v>601</v>
+      </c>
+      <c r="W73" t="s">
         <v>600</v>
-      </c>
-      <c r="V73" s="9" t="s">
-        <v>602</v>
-      </c>
-      <c r="W73" t="s">
-        <v>601</v>
       </c>
       <c r="X73">
         <v>2025</v>
@@ -5267,7 +5267,7 @@
     </row>
     <row r="74" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A74" s="28" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B74" s="49" t="s">
         <v>203</v>
@@ -5307,13 +5307,13 @@
         <v>84</v>
       </c>
       <c r="P74" s="1" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="Q74" s="9" t="s">
         <v>77</v>
       </c>
       <c r="R74" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="S74">
         <v>2023</v>
@@ -5361,13 +5361,13 @@
         <v>84</v>
       </c>
       <c r="P75" s="1" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="Q75" s="9" t="s">
         <v>77</v>
       </c>
       <c r="R75" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="S75">
         <v>2023</v>
@@ -5397,7 +5397,7 @@
       </c>
       <c r="H76" s="1"/>
       <c r="J76" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="K76" s="16" t="s">
         <v>179</v>
@@ -5406,18 +5406,18 @@
         <v>77</v>
       </c>
       <c r="M76" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="N76">
         <v>2025</v>
       </c>
       <c r="O76" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="77" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A77" s="28" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B77" s="49" t="s">
         <v>203</v>
@@ -5439,7 +5439,7 @@
       </c>
       <c r="H77" s="1"/>
       <c r="J77" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="K77" s="16" t="s">
         <v>179</v>
@@ -5448,13 +5448,13 @@
         <v>77</v>
       </c>
       <c r="M77" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="N77">
         <v>2025</v>
       </c>
       <c r="O77" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="78" spans="1:24" x14ac:dyDescent="0.2">
@@ -5476,7 +5476,7 @@
       </c>
       <c r="H78" s="1"/>
       <c r="J78" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="K78" s="16" t="s">
         <v>179</v>
@@ -5485,13 +5485,13 @@
         <v>77</v>
       </c>
       <c r="M78" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="N78">
         <v>2025</v>
       </c>
       <c r="O78" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="79" spans="1:24" x14ac:dyDescent="0.2">
@@ -5533,13 +5533,13 @@
         <v>2017</v>
       </c>
       <c r="P79" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="Q79" s="9" t="s">
+        <v>601</v>
+      </c>
+      <c r="R79" t="s">
         <v>600</v>
-      </c>
-      <c r="Q79" s="9" t="s">
-        <v>602</v>
-      </c>
-      <c r="R79" t="s">
-        <v>601</v>
       </c>
       <c r="S79">
         <v>2025</v>
@@ -5584,13 +5584,13 @@
         <v>2017</v>
       </c>
       <c r="P80" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="Q80" s="9" t="s">
+        <v>601</v>
+      </c>
+      <c r="R80" t="s">
         <v>600</v>
-      </c>
-      <c r="Q80" s="9" t="s">
-        <v>602</v>
-      </c>
-      <c r="R80" t="s">
-        <v>601</v>
       </c>
       <c r="S80">
         <v>2025</v>
@@ -5635,13 +5635,13 @@
         <v>2017</v>
       </c>
       <c r="P81" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="Q81" s="9" t="s">
+        <v>601</v>
+      </c>
+      <c r="R81" t="s">
         <v>600</v>
-      </c>
-      <c r="Q81" s="9" t="s">
-        <v>602</v>
-      </c>
-      <c r="R81" t="s">
-        <v>601</v>
       </c>
       <c r="S81">
         <v>2025</v>
@@ -5667,7 +5667,7 @@
         <v>435</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="H82" s="46"/>
       <c r="J82" s="1" t="s">
@@ -5686,13 +5686,13 @@
         <v>2017</v>
       </c>
       <c r="P82" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="Q82" s="9" t="s">
+        <v>601</v>
+      </c>
+      <c r="R82" t="s">
         <v>600</v>
-      </c>
-      <c r="Q82" s="9" t="s">
-        <v>602</v>
-      </c>
-      <c r="R82" t="s">
-        <v>601</v>
       </c>
       <c r="S82">
         <v>2025</v>
@@ -5700,7 +5700,7 @@
     </row>
     <row r="83" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A83" s="28" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B83" s="49" t="s">
         <v>203</v>
@@ -5737,13 +5737,13 @@
         <v>2017</v>
       </c>
       <c r="P83" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="Q83" s="9" t="s">
+        <v>601</v>
+      </c>
+      <c r="R83" t="s">
         <v>600</v>
-      </c>
-      <c r="Q83" s="9" t="s">
-        <v>602</v>
-      </c>
-      <c r="R83" t="s">
-        <v>601</v>
       </c>
       <c r="S83">
         <v>2025</v>
@@ -5788,13 +5788,13 @@
         <v>2017</v>
       </c>
       <c r="P84" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="Q84" s="9" t="s">
+        <v>601</v>
+      </c>
+      <c r="R84" t="s">
         <v>600</v>
-      </c>
-      <c r="Q84" s="9" t="s">
-        <v>602</v>
-      </c>
-      <c r="R84" t="s">
-        <v>601</v>
       </c>
       <c r="S84">
         <v>2025</v>
@@ -5839,13 +5839,13 @@
         <v>2017</v>
       </c>
       <c r="P85" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="Q85" s="9" t="s">
+        <v>601</v>
+      </c>
+      <c r="R85" t="s">
         <v>600</v>
-      </c>
-      <c r="Q85" s="9" t="s">
-        <v>602</v>
-      </c>
-      <c r="R85" t="s">
-        <v>601</v>
       </c>
       <c r="S85">
         <v>2025</v>
@@ -5890,13 +5890,13 @@
         <v>2017</v>
       </c>
       <c r="P86" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="Q86" s="9" t="s">
+        <v>601</v>
+      </c>
+      <c r="R86" t="s">
         <v>600</v>
-      </c>
-      <c r="Q86" s="9" t="s">
-        <v>602</v>
-      </c>
-      <c r="R86" t="s">
-        <v>601</v>
       </c>
       <c r="S86">
         <v>2025</v>
@@ -5964,7 +5964,7 @@
     </row>
     <row r="88" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A88" s="28" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B88" s="49" t="s">
         <v>203</v>
@@ -5982,7 +5982,7 @@
         <v>16</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="H88" s="1" t="b">
         <v>1</v>
@@ -6207,7 +6207,7 @@
         <v>90</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="H93" s="1"/>
       <c r="I93" s="2"/>
@@ -6292,7 +6292,7 @@
         <v>174</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H95" s="1"/>
       <c r="J95" s="1" t="s">
@@ -6358,7 +6358,7 @@
     </row>
     <row r="97" spans="1:24" s="41" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A97" s="40" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B97" s="50" t="s">
         <v>203</v>
@@ -6376,7 +6376,7 @@
         <v>173</v>
       </c>
       <c r="G97" s="41" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="J97" s="41" t="s">
         <v>116</v>
@@ -6493,7 +6493,7 @@
       </c>
       <c r="H100" s="1"/>
       <c r="J100" s="1" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="K100" s="16" t="s">
         <v>178</v>
@@ -6502,19 +6502,19 @@
         <v>77</v>
       </c>
       <c r="M100" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="N100">
         <v>2024</v>
       </c>
       <c r="P100" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="Q100" s="9" t="s">
         <v>605</v>
       </c>
-      <c r="Q100" s="9" t="s">
+      <c r="R100" t="s">
         <v>606</v>
-      </c>
-      <c r="R100" t="s">
-        <v>607</v>
       </c>
       <c r="S100">
         <v>2022</v>
@@ -6554,7 +6554,7 @@
       </c>
       <c r="H101" s="1"/>
       <c r="J101" s="1" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="K101" s="16" t="s">
         <v>178</v>
@@ -6563,19 +6563,19 @@
         <v>77</v>
       </c>
       <c r="M101" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="N101">
         <v>2024</v>
       </c>
       <c r="P101" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="Q101" s="9" t="s">
         <v>605</v>
       </c>
-      <c r="Q101" s="9" t="s">
+      <c r="R101" t="s">
         <v>606</v>
-      </c>
-      <c r="R101" t="s">
-        <v>607</v>
       </c>
       <c r="S101">
         <v>2022</v>
@@ -6614,7 +6614,7 @@
       </c>
       <c r="H102" s="1"/>
       <c r="J102" s="1" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="K102" s="16" t="s">
         <v>178</v>
@@ -6623,19 +6623,19 @@
         <v>77</v>
       </c>
       <c r="M102" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="N102">
         <v>2024</v>
       </c>
       <c r="P102" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="Q102" s="9" t="s">
         <v>605</v>
       </c>
-      <c r="Q102" s="9" t="s">
+      <c r="R102" t="s">
         <v>606</v>
-      </c>
-      <c r="R102" t="s">
-        <v>607</v>
       </c>
       <c r="S102">
         <v>2022</v>
@@ -6747,7 +6747,7 @@
     </row>
     <row r="106" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A106" s="28" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B106" s="49" t="s">
         <v>178</v>
@@ -6783,7 +6783,7 @@
     </row>
     <row r="107" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A107" s="28" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B107" s="49" t="s">
         <v>178</v>
@@ -6855,7 +6855,7 @@
     </row>
     <row r="109" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A109" s="28" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B109" s="49" t="s">
         <v>178</v>
@@ -6912,7 +6912,7 @@
       </c>
       <c r="H110" s="1"/>
       <c r="J110" s="1" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="K110" s="16" t="s">
         <v>178</v>
@@ -6921,7 +6921,7 @@
         <v>77</v>
       </c>
       <c r="M110" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="N110">
         <v>2024</v>
@@ -6960,7 +6960,7 @@
       </c>
       <c r="H111" s="1"/>
       <c r="J111" s="1" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="K111" s="16" t="s">
         <v>178</v>
@@ -6969,7 +6969,7 @@
         <v>77</v>
       </c>
       <c r="M111" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="N111">
         <v>2024</v>
@@ -6989,7 +6989,7 @@
     </row>
     <row r="112" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A112" s="28" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B112" s="49" t="s">
         <v>178</v>
@@ -7008,7 +7008,7 @@
       </c>
       <c r="H112" s="1"/>
       <c r="J112" s="1" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="K112" s="16" t="s">
         <v>178</v>
@@ -7017,7 +7017,7 @@
         <v>77</v>
       </c>
       <c r="M112" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="N112">
         <v>2024</v>
@@ -7056,7 +7056,7 @@
       </c>
       <c r="H113" s="1"/>
       <c r="J113" s="1" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="K113" s="16" t="s">
         <v>178</v>
@@ -7065,7 +7065,7 @@
         <v>77</v>
       </c>
       <c r="M113" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="N113">
         <v>2024</v>
@@ -7075,7 +7075,7 @@
     </row>
     <row r="114" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A114" s="28" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B114" s="49" t="s">
         <v>178</v>
@@ -7111,7 +7111,7 @@
     </row>
     <row r="115" spans="1:20" s="41" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A115" s="40" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B115" s="50" t="s">
         <v>178</v>
@@ -7220,7 +7220,7 @@
     </row>
     <row r="118" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="28" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B118" s="49" t="s">
         <v>178</v>
@@ -7256,7 +7256,7 @@
     </row>
     <row r="119" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="28" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B119" s="49" t="s">
         <v>178</v>
@@ -7292,7 +7292,7 @@
     </row>
     <row r="120" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A120" s="28" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B120" s="49" t="s">
         <v>178</v>
@@ -7328,7 +7328,7 @@
     </row>
     <row r="121" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A121" s="28" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B121" s="49" t="s">
         <v>178</v>
@@ -7366,7 +7366,7 @@
     </row>
     <row r="122" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A122" s="29" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B122" s="51" t="s">
         <v>178</v>
@@ -7408,7 +7408,7 @@
     </row>
     <row r="123" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="28" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B123" s="49" t="s">
         <v>179</v>
@@ -7445,24 +7445,24 @@
         <v>78</v>
       </c>
       <c r="P123" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="Q123" s="9" t="s">
         <v>77</v>
       </c>
       <c r="R123" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="S123">
         <v>2014</v>
       </c>
       <c r="T123" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="124" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="28" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B124" s="49" t="s">
         <v>179</v>
@@ -7500,34 +7500,34 @@
         <v>78</v>
       </c>
       <c r="P124" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="Q124" s="9" t="s">
         <v>77</v>
       </c>
       <c r="R124" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="S124">
         <v>2014</v>
       </c>
       <c r="T124" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="125" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="28" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B125" s="49" t="s">
         <v>179</v>
       </c>
       <c r="D125" s="49"/>
       <c r="F125" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="G125" s="1" t="s">
-        <v>476</v>
+        <v>646</v>
       </c>
       <c r="H125" s="1" t="b">
         <v>1</v>
@@ -7552,42 +7552,42 @@
         <v>78</v>
       </c>
       <c r="P125" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="Q125" s="9" t="s">
         <v>77</v>
       </c>
       <c r="R125" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="S125">
         <v>2014</v>
       </c>
       <c r="T125" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="126" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="28" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B126" s="49" t="s">
         <v>179</v>
       </c>
       <c r="D126" s="49"/>
       <c r="E126" s="14" t="s">
+        <v>476</v>
+      </c>
+      <c r="F126" t="s">
         <v>477</v>
       </c>
-      <c r="F126" t="s">
-        <v>478</v>
-      </c>
       <c r="G126" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="H126" s="1"/>
       <c r="I126" s="2"/>
       <c r="J126" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="K126" s="16" t="s">
         <v>179</v>
@@ -7596,34 +7596,34 @@
         <v>77</v>
       </c>
       <c r="M126" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="N126">
         <v>2025</v>
       </c>
       <c r="O126" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="127" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A127" s="28" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B127" s="49" t="s">
         <v>179</v>
       </c>
       <c r="D127" s="49"/>
       <c r="E127" s="14" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="F127" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="G127" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="J127" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="K127" s="16" t="s">
         <v>179</v>
@@ -7632,34 +7632,34 @@
         <v>77</v>
       </c>
       <c r="M127" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="N127">
         <v>2025</v>
       </c>
       <c r="O127" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="128" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A128" s="28" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B128" s="49" t="s">
         <v>179</v>
       </c>
       <c r="D128" s="49"/>
       <c r="E128" s="14" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="G128" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="H128" t="b">
         <v>1</v>
       </c>
       <c r="J128" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="K128" s="16" t="s">
         <v>179</v>
@@ -7668,18 +7668,18 @@
         <v>77</v>
       </c>
       <c r="M128" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="N128">
         <v>2025</v>
       </c>
       <c r="O128" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="129" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A129" s="28" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B129" s="49" t="s">
         <v>179</v>
@@ -7719,7 +7719,7 @@
         <v>78</v>
       </c>
       <c r="P129" s="1" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="Q129" s="9" t="s">
         <v>77</v>
@@ -7731,12 +7731,12 @@
         <v>2021</v>
       </c>
       <c r="T129" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="130" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A130" s="28" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B130" s="49" t="s">
         <v>179</v>
@@ -7751,7 +7751,7 @@
         <v>30</v>
       </c>
       <c r="G130" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="H130" s="1"/>
       <c r="I130" s="2"/>
@@ -7774,7 +7774,7 @@
         <v>78</v>
       </c>
       <c r="P130" s="1" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="Q130" s="9" t="s">
         <v>77</v>
@@ -7786,12 +7786,12 @@
         <v>2021</v>
       </c>
       <c r="T130" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="131" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A131" s="28" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B131" s="49" t="s">
         <v>179</v>
@@ -7806,7 +7806,7 @@
         <v>30</v>
       </c>
       <c r="G131" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="H131" s="1"/>
       <c r="I131" s="2"/>
@@ -7829,7 +7829,7 @@
         <v>78</v>
       </c>
       <c r="P131" s="1" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="Q131" s="9" t="s">
         <v>77</v>
@@ -7841,12 +7841,12 @@
         <v>2021</v>
       </c>
       <c r="T131" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="132" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A132" s="28" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B132" s="49" t="s">
         <v>179</v>
@@ -7883,13 +7883,13 @@
         <v>78</v>
       </c>
       <c r="P132" s="1" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="Q132" s="9" t="s">
         <v>86</v>
       </c>
       <c r="R132" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="S132">
         <v>2015</v>
@@ -7900,7 +7900,7 @@
     </row>
     <row r="133" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A133" s="28" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B133" s="49" t="s">
         <v>179</v>
@@ -7915,7 +7915,7 @@
         <v>130</v>
       </c>
       <c r="G133" s="1" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="H133" s="1"/>
       <c r="I133" s="2"/>
@@ -7938,13 +7938,13 @@
         <v>78</v>
       </c>
       <c r="P133" s="1" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="Q133" s="9" t="s">
         <v>86</v>
       </c>
       <c r="R133" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="S133">
         <v>2015</v>
@@ -7955,7 +7955,7 @@
     </row>
     <row r="134" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A134" s="28" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B134" s="49" t="s">
         <v>179</v>
@@ -7994,7 +7994,7 @@
     </row>
     <row r="135" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A135" s="28" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B135" s="49" t="s">
         <v>179</v>
@@ -8003,10 +8003,10 @@
         <v>165</v>
       </c>
       <c r="D135" s="49" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E135" s="14" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="F135" t="s">
         <v>131</v>
@@ -8043,7 +8043,7 @@
         <v>81</v>
       </c>
       <c r="R135" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="S135">
         <v>2016</v>
@@ -8070,7 +8070,7 @@
     </row>
     <row r="136" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A136" s="28" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B136" s="49" t="s">
         <v>179</v>
@@ -8079,16 +8079,16 @@
         <v>165</v>
       </c>
       <c r="D136" s="49" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E136" s="14" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="F136" t="s">
         <v>131</v>
       </c>
       <c r="G136" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="H136" s="1"/>
       <c r="I136" s="2"/>
@@ -8117,7 +8117,7 @@
         <v>81</v>
       </c>
       <c r="R136" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="S136">
         <v>2016</v>
@@ -8128,7 +8128,7 @@
     </row>
     <row r="137" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A137" s="28" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B137" s="49" t="s">
         <v>179</v>
@@ -8137,16 +8137,16 @@
         <v>165</v>
       </c>
       <c r="D137" s="49" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E137" s="14" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="F137" t="s">
         <v>131</v>
       </c>
       <c r="G137" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="H137" s="1"/>
       <c r="I137" s="2"/>
@@ -8175,7 +8175,7 @@
         <v>81</v>
       </c>
       <c r="R137" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="S137">
         <v>2016</v>
@@ -8186,7 +8186,7 @@
     </row>
     <row r="138" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A138" s="28" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B138" s="49" t="s">
         <v>179</v>
@@ -8195,16 +8195,16 @@
         <v>165</v>
       </c>
       <c r="D138" s="49" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E138" s="14" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="F138" t="s">
         <v>131</v>
       </c>
       <c r="G138" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H138" s="1"/>
       <c r="I138" s="2"/>
@@ -8233,7 +8233,7 @@
         <v>81</v>
       </c>
       <c r="R138" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="S138">
         <v>2016</v>
@@ -8244,7 +8244,7 @@
     </row>
     <row r="139" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A139" s="28" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B139" s="49" t="s">
         <v>179</v>
@@ -8253,10 +8253,10 @@
         <v>165</v>
       </c>
       <c r="D139" s="49" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E139" s="14" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="F139" t="s">
         <v>132</v>
@@ -8290,7 +8290,7 @@
         <v>81</v>
       </c>
       <c r="R139" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="S139">
         <v>2016</v>
@@ -8301,7 +8301,7 @@
     </row>
     <row r="140" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A140" s="28" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B140" s="49" t="s">
         <v>179</v>
@@ -8310,16 +8310,16 @@
         <v>165</v>
       </c>
       <c r="D140" s="49" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E140" s="14" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="F140" t="s">
         <v>132</v>
       </c>
       <c r="G140" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H140" s="1"/>
       <c r="J140" s="1" t="s">
@@ -8347,7 +8347,7 @@
         <v>81</v>
       </c>
       <c r="R140" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="S140">
         <v>2016</v>
@@ -8358,7 +8358,7 @@
     </row>
     <row r="141" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A141" s="28" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B141" s="49" t="s">
         <v>179</v>
@@ -8367,10 +8367,10 @@
         <v>165</v>
       </c>
       <c r="D141" s="49" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E141" s="14" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="F141" t="s">
         <v>0</v>
@@ -8404,7 +8404,7 @@
         <v>81</v>
       </c>
       <c r="R141" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="S141">
         <v>2016</v>
@@ -8415,7 +8415,7 @@
     </row>
     <row r="142" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A142" s="28" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B142" s="49" t="s">
         <v>179</v>
@@ -8424,16 +8424,16 @@
         <v>165</v>
       </c>
       <c r="D142" s="49" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E142" s="14" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="F142" t="s">
         <v>0</v>
       </c>
       <c r="G142" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="H142" s="1"/>
       <c r="J142" s="1" t="s">
@@ -8461,7 +8461,7 @@
         <v>81</v>
       </c>
       <c r="R142" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="S142">
         <v>2016</v>
@@ -8472,7 +8472,7 @@
     </row>
     <row r="143" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A143" s="28" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B143" s="49" t="s">
         <v>179</v>
@@ -8481,10 +8481,10 @@
         <v>165</v>
       </c>
       <c r="D143" s="49" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E143" s="14" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="F143" t="s">
         <v>133</v>
@@ -8518,7 +8518,7 @@
         <v>81</v>
       </c>
       <c r="R143" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="S143">
         <v>2016</v>
@@ -8529,7 +8529,7 @@
     </row>
     <row r="144" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A144" s="28" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B144" s="49" t="s">
         <v>179</v>
@@ -8538,16 +8538,16 @@
         <v>165</v>
       </c>
       <c r="D144" s="49" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E144" s="14" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="F144" t="s">
         <v>133</v>
       </c>
       <c r="G144" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="H144" s="1"/>
       <c r="J144" s="1" t="s">
@@ -8575,7 +8575,7 @@
         <v>81</v>
       </c>
       <c r="R144" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="S144">
         <v>2016</v>
@@ -8586,7 +8586,7 @@
     </row>
     <row r="145" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A145" s="28" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B145" s="49" t="s">
         <v>179</v>
@@ -8595,16 +8595,16 @@
         <v>165</v>
       </c>
       <c r="D145" s="49" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E145" s="14" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="F145" t="s">
         <v>133</v>
       </c>
       <c r="G145" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="H145" s="1"/>
       <c r="J145" s="1" t="s">
@@ -8632,7 +8632,7 @@
         <v>81</v>
       </c>
       <c r="R145" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="S145">
         <v>2016</v>
@@ -8643,7 +8643,7 @@
     </row>
     <row r="146" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A146" s="28" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B146" s="49" t="s">
         <v>179</v>
@@ -8652,7 +8652,7 @@
         <v>165</v>
       </c>
       <c r="D146" s="49" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F146" t="s">
         <v>134</v>
@@ -8682,7 +8682,7 @@
     </row>
     <row r="147" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A147" s="28" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B147" s="49" t="s">
         <v>179</v>
@@ -8691,13 +8691,13 @@
         <v>165</v>
       </c>
       <c r="D147" s="49" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F147" t="s">
         <v>134</v>
       </c>
       <c r="G147" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="J147" s="1" t="s">
         <v>114</v>
@@ -8720,7 +8720,7 @@
     </row>
     <row r="148" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A148" s="28" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B148" s="49" t="s">
         <v>179</v>
@@ -8729,13 +8729,13 @@
         <v>165</v>
       </c>
       <c r="D148" s="49" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F148" t="s">
         <v>134</v>
       </c>
       <c r="G148" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="J148" s="1" t="s">
         <v>114</v>
@@ -8758,7 +8758,7 @@
     </row>
     <row r="149" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A149" s="28" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B149" s="49" t="s">
         <v>179</v>
@@ -8800,7 +8800,7 @@
     </row>
     <row r="150" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A150" s="28" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B150" s="49" t="s">
         <v>179</v>
@@ -8834,27 +8834,27 @@
         <v>2021</v>
       </c>
       <c r="O150" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="P150" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="Q150" s="9" t="s">
         <v>77</v>
       </c>
       <c r="R150" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="S150">
         <v>2014</v>
       </c>
       <c r="T150" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="151" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A151" s="28" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B151" s="49" t="s">
         <v>179</v>
@@ -8866,10 +8866,10 @@
         <v>31</v>
       </c>
       <c r="F151" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="G151" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="H151" s="1"/>
       <c r="J151" s="1" t="s">
@@ -8888,27 +8888,27 @@
         <v>2021</v>
       </c>
       <c r="O151" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="P151" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="Q151" s="9" t="s">
         <v>77</v>
       </c>
       <c r="R151" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="S151">
         <v>2014</v>
       </c>
       <c r="T151" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="152" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A152" s="28" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B152" s="49" t="s">
         <v>179</v>
@@ -8920,10 +8920,10 @@
         <v>31</v>
       </c>
       <c r="F152" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="G152" s="1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="H152" s="1"/>
       <c r="J152" s="1" t="s">
@@ -8942,27 +8942,27 @@
         <v>2021</v>
       </c>
       <c r="O152" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="P152" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="Q152" s="9" t="s">
         <v>77</v>
       </c>
       <c r="R152" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="S152">
         <v>2014</v>
       </c>
       <c r="T152" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="153" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A153" s="28" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B153" s="49" t="s">
         <v>179</v>
@@ -8974,10 +8974,10 @@
         <v>31</v>
       </c>
       <c r="F153" t="s">
+        <v>514</v>
+      </c>
+      <c r="G153" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="G153" s="1" t="s">
-        <v>516</v>
       </c>
       <c r="H153" s="1"/>
       <c r="J153" s="1" t="s">
@@ -8996,27 +8996,27 @@
         <v>2021</v>
       </c>
       <c r="O153" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="P153" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="Q153" s="9" t="s">
         <v>77</v>
       </c>
       <c r="R153" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="S153">
         <v>2014</v>
       </c>
       <c r="T153" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="154" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A154" s="28" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B154" s="49" t="s">
         <v>179</v>
@@ -9028,10 +9028,10 @@
         <v>31</v>
       </c>
       <c r="F154" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="G154" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="H154" s="1"/>
       <c r="J154" s="1" t="s">
@@ -9050,22 +9050,22 @@
         <v>2021</v>
       </c>
       <c r="O154" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="P154" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="Q154" s="9" t="s">
         <v>77</v>
       </c>
       <c r="R154" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="S154">
         <v>2014</v>
       </c>
       <c r="T154" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="U154" s="1" t="s">
         <v>114</v>
@@ -9088,7 +9088,7 @@
     </row>
     <row r="155" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A155" s="28" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B155" s="49" t="s">
         <v>179</v>
@@ -9100,14 +9100,14 @@
         <v>31</v>
       </c>
       <c r="F155" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="G155" s="1" t="s">
         <v>49</v>
       </c>
       <c r="H155" s="1"/>
       <c r="J155" s="1" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="K155" s="16" t="s">
         <v>179</v>
@@ -9116,7 +9116,7 @@
         <v>77</v>
       </c>
       <c r="M155" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="N155">
         <v>2023</v>
@@ -9124,7 +9124,7 @@
     </row>
     <row r="156" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A156" s="28" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B156" s="49" t="s">
         <v>179</v>
@@ -9136,14 +9136,14 @@
         <v>31</v>
       </c>
       <c r="F156" t="s">
+        <v>506</v>
+      </c>
+      <c r="G156" s="1" t="s">
         <v>507</v>
-      </c>
-      <c r="G156" s="1" t="s">
-        <v>508</v>
       </c>
       <c r="H156" s="1"/>
       <c r="J156" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="K156" s="16" t="s">
         <v>179</v>
@@ -9152,18 +9152,18 @@
         <v>77</v>
       </c>
       <c r="M156" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="N156">
         <v>2025</v>
       </c>
       <c r="O156" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="157" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A157" s="28" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B157" s="49" t="s">
         <v>179</v>
@@ -9172,7 +9172,7 @@
         <v>157</v>
       </c>
       <c r="D157" s="52" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F157" t="s">
         <v>159</v>
@@ -9205,7 +9205,7 @@
     </row>
     <row r="158" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A158" s="28" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B158" s="49" t="s">
         <v>179</v>
@@ -9214,7 +9214,7 @@
         <v>157</v>
       </c>
       <c r="D158" s="52" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F158" t="s">
         <v>163</v>
@@ -9247,7 +9247,7 @@
     </row>
     <row r="159" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A159" s="28" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B159" s="49" t="s">
         <v>179</v>
@@ -9256,7 +9256,7 @@
         <v>157</v>
       </c>
       <c r="D159" s="52" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F159" t="s">
         <v>7</v>
@@ -9286,7 +9286,7 @@
     </row>
     <row r="160" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A160" s="28" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B160" s="49" t="s">
         <v>179</v>
@@ -9295,13 +9295,13 @@
         <v>157</v>
       </c>
       <c r="D160" s="52" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F160" t="s">
         <v>7</v>
       </c>
       <c r="G160" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="H160" s="1"/>
       <c r="J160" s="1" t="s">
@@ -9325,7 +9325,7 @@
     </row>
     <row r="161" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A161" s="28" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B161" s="49" t="s">
         <v>179</v>
@@ -9334,13 +9334,13 @@
         <v>157</v>
       </c>
       <c r="D161" s="52" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F161" t="s">
         <v>7</v>
       </c>
       <c r="G161" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="H161" s="1"/>
       <c r="J161" s="1" t="s">
@@ -9364,7 +9364,7 @@
     </row>
     <row r="162" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A162" s="28" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B162" s="49" t="s">
         <v>179</v>
@@ -9373,13 +9373,13 @@
         <v>157</v>
       </c>
       <c r="D162" s="52" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F162" t="s">
+        <v>526</v>
+      </c>
+      <c r="G162" s="1" t="s">
         <v>527</v>
-      </c>
-      <c r="G162" s="1" t="s">
-        <v>528</v>
       </c>
       <c r="H162" s="1"/>
       <c r="J162" s="1" t="s">
@@ -9403,7 +9403,7 @@
     </row>
     <row r="163" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A163" s="28" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B163" s="49" t="s">
         <v>179</v>
@@ -9412,7 +9412,7 @@
         <v>157</v>
       </c>
       <c r="D163" s="52" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F163" t="s">
         <v>136</v>
@@ -9457,7 +9457,7 @@
     </row>
     <row r="164" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A164" s="28" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B164" s="49" t="s">
         <v>179</v>
@@ -9466,13 +9466,13 @@
         <v>157</v>
       </c>
       <c r="D164" s="52" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F164" t="s">
         <v>136</v>
       </c>
       <c r="G164" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="H164" s="1"/>
       <c r="J164" s="1" t="s">
@@ -9496,7 +9496,7 @@
     </row>
     <row r="165" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A165" s="28" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B165" s="49" t="s">
         <v>179</v>
@@ -9505,13 +9505,13 @@
         <v>157</v>
       </c>
       <c r="D165" s="52" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F165" t="s">
         <v>136</v>
       </c>
       <c r="G165" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="H165" s="1"/>
       <c r="J165" s="1" t="s">
@@ -9535,7 +9535,7 @@
     </row>
     <row r="166" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A166" s="28" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B166" s="49" t="s">
         <v>179</v>
@@ -9547,7 +9547,7 @@
         <v>20</v>
       </c>
       <c r="E166" s="14" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="F166" t="s">
         <v>21</v>
@@ -9577,7 +9577,7 @@
     </row>
     <row r="167" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A167" s="28" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B167" s="49" t="s">
         <v>179</v>
@@ -9589,7 +9589,7 @@
         <v>20</v>
       </c>
       <c r="E167" s="14" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="F167" t="s">
         <v>22</v>
@@ -9622,7 +9622,7 @@
     </row>
     <row r="168" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A168" s="28" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B168" s="49" t="s">
         <v>179</v>
@@ -9634,13 +9634,13 @@
         <v>20</v>
       </c>
       <c r="E168" s="14" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="F168" t="s">
         <v>22</v>
       </c>
       <c r="G168" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="H168" s="1"/>
       <c r="I168" s="1"/>
@@ -9665,7 +9665,7 @@
     </row>
     <row r="169" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A169" s="28" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B169" s="49" t="s">
         <v>179</v>
@@ -9677,7 +9677,7 @@
         <v>20</v>
       </c>
       <c r="E169" s="14" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="F169" t="s">
         <v>24</v>
@@ -9707,7 +9707,7 @@
     </row>
     <row r="170" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A170" s="28" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B170" s="49" t="s">
         <v>179</v>
@@ -9719,7 +9719,7 @@
         <v>20</v>
       </c>
       <c r="E170" s="14" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="F170" t="s">
         <v>25</v>
@@ -9751,7 +9751,7 @@
     </row>
     <row r="171" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A171" s="28" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B171" s="49" t="s">
         <v>179</v>
@@ -9763,7 +9763,7 @@
         <v>20</v>
       </c>
       <c r="E171" s="14" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="F171" t="s">
         <v>26</v>
@@ -9795,7 +9795,7 @@
     </row>
     <row r="172" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A172" s="28" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B172" s="49" t="s">
         <v>179</v>
@@ -9807,7 +9807,7 @@
         <v>20</v>
       </c>
       <c r="E172" s="14" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="F172" t="s">
         <v>27</v>
@@ -9839,7 +9839,7 @@
     </row>
     <row r="173" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A173" s="28" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B173" s="49" t="s">
         <v>179</v>
@@ -9851,7 +9851,7 @@
         <v>20</v>
       </c>
       <c r="E173" s="14" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="F173" t="s">
         <v>176</v>
@@ -9881,7 +9881,7 @@
     </row>
     <row r="174" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A174" s="28" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B174" s="49" t="s">
         <v>179</v>
@@ -9893,7 +9893,7 @@
         <v>20</v>
       </c>
       <c r="E174" s="14" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="F174" t="s">
         <v>28</v>
@@ -9923,7 +9923,7 @@
     </row>
     <row r="175" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A175" s="28" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B175" s="49" t="s">
         <v>179</v>
@@ -9935,7 +9935,7 @@
         <v>20</v>
       </c>
       <c r="E175" s="14" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="F175" t="s">
         <v>29</v>
@@ -9965,7 +9965,7 @@
     </row>
     <row r="176" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A176" s="28" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B176" s="49" t="s">
         <v>179</v>
@@ -9999,12 +9999,12 @@
         <v>2021</v>
       </c>
       <c r="O176" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="177" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A177" s="28" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B177" s="49" t="s">
         <v>179</v>
@@ -10019,7 +10019,7 @@
         <v>166</v>
       </c>
       <c r="G177" s="1" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="H177" s="1"/>
       <c r="J177" s="1" t="s">
@@ -10038,12 +10038,12 @@
         <v>2021</v>
       </c>
       <c r="O177" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="178" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A178" s="28" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B178" s="49" t="s">
         <v>179</v>
@@ -10058,7 +10058,7 @@
         <v>166</v>
       </c>
       <c r="G178" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H178" s="1"/>
       <c r="J178" s="1" t="s">
@@ -10077,12 +10077,12 @@
         <v>2021</v>
       </c>
       <c r="O178" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="179" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A179" s="28" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B179" s="49" t="s">
         <v>179</v>
@@ -10097,7 +10097,7 @@
         <v>166</v>
       </c>
       <c r="G179" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H179" s="1"/>
       <c r="J179" s="1" t="s">
@@ -10116,12 +10116,12 @@
         <v>2021</v>
       </c>
       <c r="O179" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="180" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A180" s="28" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B180" s="49" t="s">
         <v>179</v>
@@ -10136,7 +10136,7 @@
         <v>166</v>
       </c>
       <c r="G180" s="1" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="H180" s="1" t="b">
         <v>1</v>
@@ -10157,12 +10157,12 @@
         <v>2021</v>
       </c>
       <c r="O180" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="181" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A181" s="28" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B181" s="49" t="s">
         <v>179</v>
@@ -10174,7 +10174,7 @@
         <v>158</v>
       </c>
       <c r="F181" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="G181" s="1" t="s">
         <v>167</v>
@@ -10201,7 +10201,7 @@
     </row>
     <row r="182" spans="1:15" x14ac:dyDescent="0.2">
       <c r="G182" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="J182" s="1" t="s">
         <v>201</v>
@@ -10646,7 +10646,7 @@
         <v>75</v>
       </c>
       <c r="B1" s="53" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C1" s="66" t="s">
         <v>127</v>
@@ -10667,10 +10667,10 @@
         <v>126</v>
       </c>
       <c r="I1" s="68" t="s">
+        <v>570</v>
+      </c>
+      <c r="J1" s="68" t="s">
         <v>571</v>
-      </c>
-      <c r="J1" s="68" t="s">
-        <v>572</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -10681,7 +10681,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="65" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D2" s="48" t="s">
         <v>177</v>
@@ -10690,7 +10690,7 @@
         <v>215</v>
       </c>
       <c r="F2" s="59" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="G2" s="59"/>
       <c r="H2" s="59"/>
@@ -10698,7 +10698,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="54" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -10709,16 +10709,16 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="D3" s="48" t="s">
         <v>216</v>
       </c>
       <c r="E3" s="59" t="s">
+        <v>597</v>
+      </c>
+      <c r="F3" s="59" t="s">
         <v>598</v>
-      </c>
-      <c r="F3" s="59" t="s">
-        <v>599</v>
       </c>
       <c r="G3" s="59">
         <v>2023</v>
@@ -10735,7 +10735,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="65" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D4" s="48" t="s">
         <v>179</v>
@@ -10744,13 +10744,13 @@
         <v>77</v>
       </c>
       <c r="F4" s="59" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="G4" s="59">
         <v>2025</v>
       </c>
       <c r="H4" s="59" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="I4" s="59"/>
       <c r="J4" s="59"/>
@@ -10763,7 +10763,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D5" s="48" t="s">
         <v>178</v>
@@ -10772,7 +10772,7 @@
         <v>77</v>
       </c>
       <c r="F5" s="59" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="G5" s="59">
         <v>2024</v>
@@ -10815,16 +10815,16 @@
         <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="D7" s="48" t="s">
         <v>178</v>
       </c>
       <c r="E7" s="69" t="s">
+        <v>605</v>
+      </c>
+      <c r="F7" s="59" t="s">
         <v>606</v>
-      </c>
-      <c r="F7" s="59" t="s">
-        <v>607</v>
       </c>
       <c r="G7" s="59">
         <v>2022</v>

</xml_diff>